<commit_message>
debug of alpha version of v_select.py completed
</commit_message>
<xml_diff>
--- a/src/databases/Vessel_Database_python.xlsx
+++ b/src/databases/Vessel_Database_python.xlsx
@@ -856,7 +856,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="569">
   <si>
     <t>Source of information</t>
   </si>
@@ -2646,13 +2646,46 @@
     <t>Vessel description</t>
   </si>
   <si>
-    <t>Beam</t>
-  </si>
-  <si>
-    <t>Deck Space [m2]</t>
-  </si>
-  <si>
-    <t>Deck Loading [ton/m2]</t>
+    <t>Vessel class</t>
+  </si>
+  <si>
+    <t>Vessel type</t>
+  </si>
+  <si>
+    <t>Year built</t>
+  </si>
+  <si>
+    <t>Last converted</t>
+  </si>
+  <si>
+    <t>Gross tonnage [ton]</t>
+  </si>
+  <si>
+    <t>Length [m]</t>
+  </si>
+  <si>
+    <t>Beam [m]</t>
+  </si>
+  <si>
+    <t>Min. draft [m]</t>
+  </si>
+  <si>
+    <t>Max. draft [m]</t>
+  </si>
+  <si>
+    <t>Deck space [m2]</t>
+  </si>
+  <si>
+    <t>Deck loading [ton/m2]</t>
+  </si>
+  <si>
+    <t>Max. cargo [ton]</t>
+  </si>
+  <si>
+    <t>Heli diamter</t>
+  </si>
+  <si>
+    <t>Heli tonnage</t>
   </si>
 </sst>
 </file>
@@ -3437,6 +3470,24 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3446,23 +3497,86 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3504,87 +3618,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3915,48 +3948,48 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="101" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="95"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="95"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="95"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="95"/>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="101"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="101"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B7" s="95"/>
-      <c r="C7" s="95"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="95"/>
-      <c r="F7" s="95"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="101"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="95"/>
-      <c r="C8" s="95"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="95"/>
-      <c r="F8" s="95"/>
+      <c r="B8" s="101"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="101"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="95"/>
-      <c r="C9" s="95"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="95"/>
-      <c r="F9" s="95"/>
+      <c r="B9" s="101"/>
+      <c r="C9" s="101"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="17"/>
@@ -3974,10 +4007,10 @@
     </row>
     <row r="12" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="2:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="96" t="s">
+      <c r="B13" s="102" t="s">
         <v>175</v>
       </c>
-      <c r="C13" s="97"/>
+      <c r="C13" s="103"/>
       <c r="D13" s="32"/>
     </row>
     <row r="14" spans="2:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -4014,10 +4047,10 @@
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="98" t="s">
+      <c r="B17" s="95" t="s">
         <v>165</v>
       </c>
-      <c r="C17" s="101" t="s">
+      <c r="C17" s="97" t="s">
         <v>164</v>
       </c>
       <c r="D17" s="22" t="s">
@@ -4026,23 +4059,23 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="99"/>
-      <c r="C18" s="102"/>
+      <c r="C18" s="100"/>
       <c r="D18" s="22" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="100"/>
-      <c r="C19" s="103"/>
+      <c r="B19" s="96"/>
+      <c r="C19" s="98"/>
       <c r="D19" s="23" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="98" t="s">
+      <c r="B20" s="95" t="s">
         <v>160</v>
       </c>
-      <c r="C20" s="101" t="s">
+      <c r="C20" s="97" t="s">
         <v>159</v>
       </c>
       <c r="D20" s="22" t="s">
@@ -4050,17 +4083,17 @@
       </c>
     </row>
     <row r="21" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="100"/>
-      <c r="C21" s="103"/>
+      <c r="B21" s="96"/>
+      <c r="C21" s="98"/>
       <c r="D21" s="23" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B22" s="98" t="s">
+      <c r="B22" s="95" t="s">
         <v>156</v>
       </c>
-      <c r="C22" s="101" t="s">
+      <c r="C22" s="97" t="s">
         <v>155</v>
       </c>
       <c r="D22" s="22" t="s">
@@ -4068,17 +4101,17 @@
       </c>
     </row>
     <row r="23" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="100"/>
-      <c r="C23" s="103"/>
+      <c r="B23" s="96"/>
+      <c r="C23" s="98"/>
       <c r="D23" s="23" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B24" s="98" t="s">
+      <c r="B24" s="95" t="s">
         <v>152</v>
       </c>
-      <c r="C24" s="101" t="s">
+      <c r="C24" s="97" t="s">
         <v>151</v>
       </c>
       <c r="D24" s="22" t="s">
@@ -4087,23 +4120,23 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25" s="99"/>
-      <c r="C25" s="102"/>
+      <c r="C25" s="100"/>
       <c r="D25" s="22" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="100"/>
-      <c r="C26" s="103"/>
+      <c r="B26" s="96"/>
+      <c r="C26" s="98"/>
       <c r="D26" s="23" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="98" t="s">
+      <c r="B27" s="95" t="s">
         <v>147</v>
       </c>
-      <c r="C27" s="101" t="s">
+      <c r="C27" s="97" t="s">
         <v>146</v>
       </c>
       <c r="D27" s="28" t="s">
@@ -4111,17 +4144,17 @@
       </c>
     </row>
     <row r="28" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="100"/>
-      <c r="C28" s="103"/>
+      <c r="B28" s="96"/>
+      <c r="C28" s="98"/>
       <c r="D28" s="27" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B29" s="98" t="s">
+      <c r="B29" s="95" t="s">
         <v>143</v>
       </c>
-      <c r="C29" s="101" t="s">
+      <c r="C29" s="97" t="s">
         <v>142</v>
       </c>
       <c r="D29" s="22" t="s">
@@ -4130,14 +4163,14 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" s="99"/>
-      <c r="C30" s="102"/>
+      <c r="C30" s="100"/>
       <c r="D30" s="22" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="100"/>
-      <c r="C31" s="103"/>
+      <c r="B31" s="96"/>
+      <c r="C31" s="98"/>
       <c r="D31" s="23" t="s">
         <v>139</v>
       </c>
@@ -4154,10 +4187,10 @@
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="98" t="s">
+      <c r="B33" s="95" t="s">
         <v>135</v>
       </c>
-      <c r="C33" s="101" t="s">
+      <c r="C33" s="97" t="s">
         <v>134</v>
       </c>
       <c r="D33" s="24" t="s">
@@ -4166,23 +4199,23 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B34" s="99"/>
-      <c r="C34" s="102"/>
+      <c r="C34" s="100"/>
       <c r="D34" s="22" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="100"/>
-      <c r="C35" s="103"/>
+      <c r="B35" s="96"/>
+      <c r="C35" s="98"/>
       <c r="D35" s="23" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B36" s="98" t="s">
+      <c r="B36" s="95" t="s">
         <v>130</v>
       </c>
-      <c r="C36" s="101" t="s">
+      <c r="C36" s="97" t="s">
         <v>129</v>
       </c>
       <c r="D36" s="22" t="s">
@@ -4190,17 +4223,17 @@
       </c>
     </row>
     <row r="37" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="100"/>
-      <c r="C37" s="103"/>
+      <c r="B37" s="96"/>
+      <c r="C37" s="98"/>
       <c r="D37" s="23" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B38" s="98" t="s">
+      <c r="B38" s="95" t="s">
         <v>126</v>
       </c>
-      <c r="C38" s="101" t="s">
+      <c r="C38" s="97" t="s">
         <v>125</v>
       </c>
       <c r="D38" s="22" t="s">
@@ -4208,17 +4241,17 @@
       </c>
     </row>
     <row r="39" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="100"/>
-      <c r="C39" s="103"/>
+      <c r="B39" s="96"/>
+      <c r="C39" s="98"/>
       <c r="D39" s="23" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B40" s="98" t="s">
+      <c r="B40" s="95" t="s">
         <v>122</v>
       </c>
-      <c r="C40" s="101" t="s">
+      <c r="C40" s="97" t="s">
         <v>121</v>
       </c>
       <c r="D40" s="22" t="s">
@@ -4226,17 +4259,17 @@
       </c>
     </row>
     <row r="41" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="100"/>
-      <c r="C41" s="103"/>
+      <c r="B41" s="96"/>
+      <c r="C41" s="98"/>
       <c r="D41" s="23" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B42" s="98" t="s">
+      <c r="B42" s="95" t="s">
         <v>118</v>
       </c>
-      <c r="C42" s="101" t="s">
+      <c r="C42" s="97" t="s">
         <v>117</v>
       </c>
       <c r="D42" s="22" t="s">
@@ -4245,23 +4278,23 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B43" s="99"/>
-      <c r="C43" s="102"/>
+      <c r="C43" s="100"/>
       <c r="D43" s="22" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="100"/>
-      <c r="C44" s="103"/>
+      <c r="B44" s="96"/>
+      <c r="C44" s="98"/>
       <c r="D44" s="23" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="98" t="s">
+      <c r="B45" s="95" t="s">
         <v>113</v>
       </c>
-      <c r="C45" s="101" t="s">
+      <c r="C45" s="97" t="s">
         <v>112</v>
       </c>
       <c r="D45" s="22" t="s">
@@ -4270,14 +4303,14 @@
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B46" s="99"/>
-      <c r="C46" s="102"/>
+      <c r="C46" s="100"/>
       <c r="D46" s="22" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="100"/>
-      <c r="C47" s="103"/>
+      <c r="B47" s="96"/>
+      <c r="C47" s="98"/>
       <c r="D47" s="21" t="s">
         <v>109</v>
       </c>
@@ -4298,6 +4331,24 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B4:F9"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="B45:B47"/>
@@ -4306,24 +4357,6 @@
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="C42:C44"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="B4:F9"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4377,369 +4410,369 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:90" ht="33.5" x14ac:dyDescent="0.35">
-      <c r="B1" s="120" t="s">
+      <c r="B1" s="121" t="s">
         <v>177</v>
       </c>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="120"/>
-      <c r="L1" s="120"/>
-      <c r="M1" s="120"/>
-      <c r="N1" s="120"/>
-      <c r="O1" s="120"/>
-      <c r="P1" s="120"/>
-      <c r="Q1" s="120"/>
-      <c r="R1" s="120"/>
-      <c r="S1" s="120"/>
-      <c r="T1" s="120"/>
-      <c r="U1" s="120"/>
-      <c r="V1" s="120"/>
-      <c r="W1" s="120"/>
-      <c r="X1" s="120"/>
-      <c r="Y1" s="120"/>
-      <c r="Z1" s="120"/>
-      <c r="AA1" s="120"/>
-      <c r="AB1" s="120"/>
-      <c r="AC1" s="120"/>
-      <c r="AD1" s="120"/>
-      <c r="AE1" s="120"/>
-      <c r="AF1" s="120"/>
-      <c r="AG1" s="120"/>
-      <c r="AH1" s="120"/>
-      <c r="AI1" s="120"/>
-      <c r="AJ1" s="120"/>
-      <c r="AK1" s="120"/>
-      <c r="AL1" s="120"/>
-      <c r="AM1" s="120"/>
-      <c r="AN1" s="120"/>
-      <c r="AO1" s="120"/>
-      <c r="AP1" s="120"/>
-      <c r="AQ1" s="120"/>
-      <c r="AR1" s="120"/>
-      <c r="AS1" s="120"/>
-      <c r="AT1" s="120"/>
-      <c r="AU1" s="120"/>
-      <c r="AV1" s="120"/>
-      <c r="AW1" s="120"/>
-      <c r="AX1" s="120"/>
-      <c r="AY1" s="120"/>
-      <c r="AZ1" s="120"/>
-      <c r="BA1" s="120"/>
-      <c r="BB1" s="120"/>
-      <c r="BC1" s="120"/>
-      <c r="BD1" s="120"/>
-      <c r="BE1" s="120"/>
-      <c r="BF1" s="120"/>
-      <c r="BG1" s="120"/>
-      <c r="BH1" s="120"/>
-      <c r="BI1" s="120"/>
-      <c r="BJ1" s="120"/>
-      <c r="BK1" s="120"/>
-      <c r="BL1" s="120"/>
-      <c r="BM1" s="120"/>
-      <c r="BN1" s="120"/>
-      <c r="BO1" s="120"/>
-      <c r="BP1" s="120"/>
-      <c r="BQ1" s="120"/>
-      <c r="BR1" s="120"/>
-      <c r="BS1" s="120"/>
-      <c r="BT1" s="120"/>
-      <c r="BU1" s="120"/>
-      <c r="BV1" s="120"/>
-      <c r="BW1" s="120"/>
-      <c r="BX1" s="120"/>
-      <c r="BY1" s="120"/>
-      <c r="BZ1" s="120"/>
-      <c r="CA1" s="120"/>
-      <c r="CB1" s="120"/>
-      <c r="CC1" s="120"/>
-      <c r="CD1" s="120"/>
-      <c r="CE1" s="120"/>
-      <c r="CF1" s="120"/>
-      <c r="CG1" s="120"/>
-      <c r="CH1" s="120"/>
-      <c r="CI1" s="120"/>
-      <c r="CJ1" s="120"/>
-      <c r="CK1" s="120"/>
-      <c r="CL1" s="120"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="121"/>
+      <c r="O1" s="121"/>
+      <c r="P1" s="121"/>
+      <c r="Q1" s="121"/>
+      <c r="R1" s="121"/>
+      <c r="S1" s="121"/>
+      <c r="T1" s="121"/>
+      <c r="U1" s="121"/>
+      <c r="V1" s="121"/>
+      <c r="W1" s="121"/>
+      <c r="X1" s="121"/>
+      <c r="Y1" s="121"/>
+      <c r="Z1" s="121"/>
+      <c r="AA1" s="121"/>
+      <c r="AB1" s="121"/>
+      <c r="AC1" s="121"/>
+      <c r="AD1" s="121"/>
+      <c r="AE1" s="121"/>
+      <c r="AF1" s="121"/>
+      <c r="AG1" s="121"/>
+      <c r="AH1" s="121"/>
+      <c r="AI1" s="121"/>
+      <c r="AJ1" s="121"/>
+      <c r="AK1" s="121"/>
+      <c r="AL1" s="121"/>
+      <c r="AM1" s="121"/>
+      <c r="AN1" s="121"/>
+      <c r="AO1" s="121"/>
+      <c r="AP1" s="121"/>
+      <c r="AQ1" s="121"/>
+      <c r="AR1" s="121"/>
+      <c r="AS1" s="121"/>
+      <c r="AT1" s="121"/>
+      <c r="AU1" s="121"/>
+      <c r="AV1" s="121"/>
+      <c r="AW1" s="121"/>
+      <c r="AX1" s="121"/>
+      <c r="AY1" s="121"/>
+      <c r="AZ1" s="121"/>
+      <c r="BA1" s="121"/>
+      <c r="BB1" s="121"/>
+      <c r="BC1" s="121"/>
+      <c r="BD1" s="121"/>
+      <c r="BE1" s="121"/>
+      <c r="BF1" s="121"/>
+      <c r="BG1" s="121"/>
+      <c r="BH1" s="121"/>
+      <c r="BI1" s="121"/>
+      <c r="BJ1" s="121"/>
+      <c r="BK1" s="121"/>
+      <c r="BL1" s="121"/>
+      <c r="BM1" s="121"/>
+      <c r="BN1" s="121"/>
+      <c r="BO1" s="121"/>
+      <c r="BP1" s="121"/>
+      <c r="BQ1" s="121"/>
+      <c r="BR1" s="121"/>
+      <c r="BS1" s="121"/>
+      <c r="BT1" s="121"/>
+      <c r="BU1" s="121"/>
+      <c r="BV1" s="121"/>
+      <c r="BW1" s="121"/>
+      <c r="BX1" s="121"/>
+      <c r="BY1" s="121"/>
+      <c r="BZ1" s="121"/>
+      <c r="CA1" s="121"/>
+      <c r="CB1" s="121"/>
+      <c r="CC1" s="121"/>
+      <c r="CD1" s="121"/>
+      <c r="CE1" s="121"/>
+      <c r="CF1" s="121"/>
+      <c r="CG1" s="121"/>
+      <c r="CH1" s="121"/>
+      <c r="CI1" s="121"/>
+      <c r="CJ1" s="121"/>
+      <c r="CK1" s="121"/>
+      <c r="CL1" s="121"/>
     </row>
     <row r="2" spans="1:90" s="42" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="43"/>
-      <c r="C2" s="123" t="s">
+      <c r="C2" s="122" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="124"/>
-      <c r="L2" s="125"/>
-      <c r="M2" s="132" t="s">
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="124"/>
+      <c r="M2" s="109" t="s">
         <v>65</v>
       </c>
-      <c r="N2" s="133"/>
-      <c r="O2" s="133"/>
-      <c r="P2" s="133"/>
-      <c r="Q2" s="133"/>
-      <c r="R2" s="133"/>
-      <c r="S2" s="133"/>
-      <c r="T2" s="133"/>
-      <c r="U2" s="133"/>
-      <c r="V2" s="133"/>
-      <c r="W2" s="133"/>
-      <c r="X2" s="133"/>
-      <c r="Y2" s="133"/>
-      <c r="Z2" s="133"/>
-      <c r="AA2" s="133"/>
-      <c r="AB2" s="133"/>
-      <c r="AC2" s="133"/>
-      <c r="AD2" s="134"/>
-      <c r="AE2" s="126" t="s">
+      <c r="N2" s="110"/>
+      <c r="O2" s="110"/>
+      <c r="P2" s="110"/>
+      <c r="Q2" s="110"/>
+      <c r="R2" s="110"/>
+      <c r="S2" s="110"/>
+      <c r="T2" s="110"/>
+      <c r="U2" s="110"/>
+      <c r="V2" s="110"/>
+      <c r="W2" s="110"/>
+      <c r="X2" s="110"/>
+      <c r="Y2" s="110"/>
+      <c r="Z2" s="110"/>
+      <c r="AA2" s="110"/>
+      <c r="AB2" s="110"/>
+      <c r="AC2" s="110"/>
+      <c r="AD2" s="111"/>
+      <c r="AE2" s="125" t="s">
         <v>178</v>
       </c>
-      <c r="AF2" s="126"/>
-      <c r="AG2" s="126"/>
-      <c r="AH2" s="126"/>
-      <c r="AI2" s="104" t="s">
+      <c r="AF2" s="125"/>
+      <c r="AG2" s="125"/>
+      <c r="AH2" s="125"/>
+      <c r="AI2" s="131" t="s">
         <v>103</v>
       </c>
-      <c r="AJ2" s="105"/>
-      <c r="AK2" s="105"/>
-      <c r="AL2" s="105"/>
-      <c r="AM2" s="105"/>
-      <c r="AN2" s="105"/>
-      <c r="AO2" s="105"/>
-      <c r="AP2" s="105"/>
-      <c r="AQ2" s="105"/>
-      <c r="AR2" s="105"/>
-      <c r="AS2" s="105"/>
-      <c r="AT2" s="105"/>
-      <c r="AU2" s="105"/>
-      <c r="AV2" s="105"/>
-      <c r="AW2" s="105"/>
-      <c r="AX2" s="105"/>
-      <c r="AY2" s="105"/>
-      <c r="AZ2" s="105"/>
-      <c r="BA2" s="105"/>
-      <c r="BB2" s="105"/>
-      <c r="BC2" s="105"/>
-      <c r="BD2" s="105"/>
-      <c r="BE2" s="105"/>
-      <c r="BF2" s="105"/>
-      <c r="BG2" s="105"/>
-      <c r="BH2" s="105"/>
-      <c r="BI2" s="105"/>
-      <c r="BJ2" s="105"/>
-      <c r="BK2" s="105"/>
-      <c r="BL2" s="105"/>
-      <c r="BM2" s="105"/>
-      <c r="BN2" s="105"/>
-      <c r="BO2" s="105"/>
-      <c r="BP2" s="105"/>
-      <c r="BQ2" s="105"/>
-      <c r="BR2" s="105"/>
-      <c r="BS2" s="105"/>
-      <c r="BT2" s="106" t="s">
+      <c r="AJ2" s="132"/>
+      <c r="AK2" s="132"/>
+      <c r="AL2" s="132"/>
+      <c r="AM2" s="132"/>
+      <c r="AN2" s="132"/>
+      <c r="AO2" s="132"/>
+      <c r="AP2" s="132"/>
+      <c r="AQ2" s="132"/>
+      <c r="AR2" s="132"/>
+      <c r="AS2" s="132"/>
+      <c r="AT2" s="132"/>
+      <c r="AU2" s="132"/>
+      <c r="AV2" s="132"/>
+      <c r="AW2" s="132"/>
+      <c r="AX2" s="132"/>
+      <c r="AY2" s="132"/>
+      <c r="AZ2" s="132"/>
+      <c r="BA2" s="132"/>
+      <c r="BB2" s="132"/>
+      <c r="BC2" s="132"/>
+      <c r="BD2" s="132"/>
+      <c r="BE2" s="132"/>
+      <c r="BF2" s="132"/>
+      <c r="BG2" s="132"/>
+      <c r="BH2" s="132"/>
+      <c r="BI2" s="132"/>
+      <c r="BJ2" s="132"/>
+      <c r="BK2" s="132"/>
+      <c r="BL2" s="132"/>
+      <c r="BM2" s="132"/>
+      <c r="BN2" s="132"/>
+      <c r="BO2" s="132"/>
+      <c r="BP2" s="132"/>
+      <c r="BQ2" s="132"/>
+      <c r="BR2" s="132"/>
+      <c r="BS2" s="132"/>
+      <c r="BT2" s="133" t="s">
         <v>59</v>
       </c>
-      <c r="BU2" s="106"/>
-      <c r="BV2" s="106"/>
-      <c r="BW2" s="106"/>
-      <c r="BX2" s="106"/>
-      <c r="BY2" s="106"/>
-      <c r="BZ2" s="106"/>
-      <c r="CA2" s="106"/>
-      <c r="CB2" s="106"/>
-      <c r="CC2" s="107" t="s">
+      <c r="BU2" s="133"/>
+      <c r="BV2" s="133"/>
+      <c r="BW2" s="133"/>
+      <c r="BX2" s="133"/>
+      <c r="BY2" s="133"/>
+      <c r="BZ2" s="133"/>
+      <c r="CA2" s="133"/>
+      <c r="CB2" s="133"/>
+      <c r="CC2" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="CD2" s="107"/>
-      <c r="CE2" s="107"/>
-      <c r="CF2" s="107"/>
-      <c r="CG2" s="108" t="s">
+      <c r="CD2" s="134"/>
+      <c r="CE2" s="134"/>
+      <c r="CF2" s="134"/>
+      <c r="CG2" s="135" t="s">
         <v>1</v>
       </c>
-      <c r="CH2" s="108"/>
-      <c r="CI2" s="108"/>
-      <c r="CJ2" s="108"/>
+      <c r="CH2" s="135"/>
+      <c r="CI2" s="135"/>
+      <c r="CJ2" s="135"/>
     </row>
     <row r="3" spans="1:90" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="128" t="s">
+      <c r="B3" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="127" t="s">
+      <c r="C3" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="129" t="s">
+      <c r="D3" s="128" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="127" t="s">
+      <c r="E3" s="126" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="127" t="s">
+      <c r="F3" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="127" t="s">
+      <c r="G3" s="126" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="131" t="s">
+      <c r="H3" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="127" t="s">
+      <c r="I3" s="126" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="127" t="s">
+      <c r="J3" s="126" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="127" t="s">
+      <c r="K3" s="126" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="127" t="s">
+      <c r="L3" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="121" t="s">
+      <c r="M3" s="118" t="s">
         <v>46</v>
       </c>
-      <c r="N3" s="141" t="s">
+      <c r="N3" s="108" t="s">
         <v>57</v>
       </c>
-      <c r="O3" s="141"/>
-      <c r="P3" s="141" t="s">
+      <c r="O3" s="108"/>
+      <c r="P3" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" s="141"/>
-      <c r="R3" s="121" t="s">
+      <c r="Q3" s="108"/>
+      <c r="R3" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="121" t="s">
+      <c r="S3" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="T3" s="121" t="s">
+      <c r="T3" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="U3" s="139" t="s">
+      <c r="U3" s="116" t="s">
         <v>66</v>
       </c>
-      <c r="V3" s="140"/>
-      <c r="W3" s="142"/>
-      <c r="X3" s="139" t="s">
+      <c r="V3" s="117"/>
+      <c r="W3" s="120"/>
+      <c r="X3" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="Y3" s="140"/>
+      <c r="Y3" s="117"/>
       <c r="Z3" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="AA3" s="143" t="s">
+      <c r="AA3" s="106" t="s">
         <v>98</v>
       </c>
-      <c r="AB3" s="144"/>
-      <c r="AC3" s="135" t="s">
+      <c r="AB3" s="107"/>
+      <c r="AC3" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="AD3" s="136"/>
-      <c r="AE3" s="137" t="s">
+      <c r="AD3" s="113"/>
+      <c r="AE3" s="114" t="s">
         <v>47</v>
       </c>
-      <c r="AF3" s="137" t="s">
+      <c r="AF3" s="114" t="s">
         <v>201</v>
       </c>
-      <c r="AG3" s="137" t="s">
+      <c r="AG3" s="114" t="s">
         <v>202</v>
       </c>
-      <c r="AH3" s="137" t="s">
+      <c r="AH3" s="114" t="s">
         <v>203</v>
       </c>
-      <c r="AI3" s="115" t="s">
+      <c r="AI3" s="142" t="s">
         <v>63</v>
       </c>
-      <c r="AJ3" s="116"/>
-      <c r="AK3" s="116"/>
-      <c r="AL3" s="116"/>
-      <c r="AM3" s="117"/>
-      <c r="AN3" s="115" t="s">
+      <c r="AJ3" s="143"/>
+      <c r="AK3" s="143"/>
+      <c r="AL3" s="143"/>
+      <c r="AM3" s="144"/>
+      <c r="AN3" s="142" t="s">
         <v>60</v>
       </c>
-      <c r="AO3" s="116"/>
-      <c r="AP3" s="116"/>
-      <c r="AQ3" s="117"/>
-      <c r="AR3" s="115" t="s">
+      <c r="AO3" s="143"/>
+      <c r="AP3" s="143"/>
+      <c r="AQ3" s="144"/>
+      <c r="AR3" s="142" t="s">
         <v>73</v>
       </c>
-      <c r="AS3" s="116"/>
-      <c r="AT3" s="116"/>
+      <c r="AS3" s="143"/>
+      <c r="AT3" s="143"/>
       <c r="AU3" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="AV3" s="109" t="s">
+      <c r="AV3" s="136" t="s">
         <v>102</v>
       </c>
-      <c r="AW3" s="110"/>
-      <c r="AX3" s="111"/>
-      <c r="AY3" s="109" t="s">
+      <c r="AW3" s="137"/>
+      <c r="AX3" s="138"/>
+      <c r="AY3" s="136" t="s">
         <v>80</v>
       </c>
-      <c r="AZ3" s="110"/>
-      <c r="BA3" s="111"/>
-      <c r="BB3" s="109" t="s">
+      <c r="AZ3" s="137"/>
+      <c r="BA3" s="138"/>
+      <c r="BB3" s="136" t="s">
         <v>85</v>
       </c>
-      <c r="BC3" s="110"/>
-      <c r="BD3" s="110"/>
-      <c r="BE3" s="110"/>
-      <c r="BF3" s="110"/>
-      <c r="BG3" s="110"/>
-      <c r="BH3" s="110"/>
-      <c r="BI3" s="110"/>
-      <c r="BJ3" s="110"/>
-      <c r="BK3" s="111"/>
-      <c r="BL3" s="109" t="s">
+      <c r="BC3" s="137"/>
+      <c r="BD3" s="137"/>
+      <c r="BE3" s="137"/>
+      <c r="BF3" s="137"/>
+      <c r="BG3" s="137"/>
+      <c r="BH3" s="137"/>
+      <c r="BI3" s="137"/>
+      <c r="BJ3" s="137"/>
+      <c r="BK3" s="138"/>
+      <c r="BL3" s="136" t="s">
         <v>205</v>
       </c>
-      <c r="BM3" s="110"/>
-      <c r="BN3" s="110"/>
-      <c r="BO3" s="110"/>
-      <c r="BP3" s="110"/>
-      <c r="BQ3" s="109" t="s">
+      <c r="BM3" s="137"/>
+      <c r="BN3" s="137"/>
+      <c r="BO3" s="137"/>
+      <c r="BP3" s="137"/>
+      <c r="BQ3" s="136" t="s">
         <v>86</v>
       </c>
-      <c r="BR3" s="110"/>
-      <c r="BS3" s="110"/>
-      <c r="BT3" s="112" t="s">
+      <c r="BR3" s="137"/>
+      <c r="BS3" s="137"/>
+      <c r="BT3" s="139" t="s">
         <v>180</v>
       </c>
-      <c r="BU3" s="113"/>
-      <c r="BV3" s="112" t="s">
+      <c r="BU3" s="140"/>
+      <c r="BV3" s="139" t="s">
         <v>181</v>
       </c>
-      <c r="BW3" s="114"/>
-      <c r="BX3" s="114"/>
-      <c r="BY3" s="112" t="s">
+      <c r="BW3" s="141"/>
+      <c r="BX3" s="141"/>
+      <c r="BY3" s="139" t="s">
         <v>182</v>
       </c>
-      <c r="BZ3" s="114"/>
-      <c r="CA3" s="113"/>
+      <c r="BZ3" s="141"/>
+      <c r="CA3" s="140"/>
       <c r="CB3" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="CC3" s="118" t="s">
+      <c r="CC3" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="CD3" s="118" t="s">
+      <c r="CD3" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="CE3" s="118" t="s">
+      <c r="CE3" s="104" t="s">
         <v>18</v>
       </c>
-      <c r="CF3" s="118" t="s">
+      <c r="CF3" s="104" t="s">
         <v>19</v>
       </c>
       <c r="CG3" s="12"/>
@@ -4749,18 +4782,18 @@
     </row>
     <row r="4" spans="1:90" ht="134.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
-      <c r="B4" s="128"/>
-      <c r="C4" s="127"/>
-      <c r="D4" s="130"/>
-      <c r="E4" s="127"/>
-      <c r="F4" s="127"/>
-      <c r="G4" s="127"/>
-      <c r="H4" s="131"/>
-      <c r="I4" s="127"/>
-      <c r="J4" s="127"/>
-      <c r="K4" s="127"/>
-      <c r="L4" s="127"/>
-      <c r="M4" s="122"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="126"/>
+      <c r="H4" s="130"/>
+      <c r="I4" s="126"/>
+      <c r="J4" s="126"/>
+      <c r="K4" s="126"/>
+      <c r="L4" s="126"/>
+      <c r="M4" s="119"/>
       <c r="N4" s="2" t="s">
         <v>40</v>
       </c>
@@ -4773,9 +4806,9 @@
       <c r="Q4" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="R4" s="122"/>
-      <c r="S4" s="122"/>
-      <c r="T4" s="122"/>
+      <c r="R4" s="119"/>
+      <c r="S4" s="119"/>
+      <c r="T4" s="119"/>
       <c r="U4" s="2" t="s">
         <v>42</v>
       </c>
@@ -4806,10 +4839,10 @@
       <c r="AD4" s="35" t="s">
         <v>216</v>
       </c>
-      <c r="AE4" s="138"/>
-      <c r="AF4" s="138"/>
-      <c r="AG4" s="138"/>
-      <c r="AH4" s="138"/>
+      <c r="AE4" s="115"/>
+      <c r="AF4" s="115"/>
+      <c r="AG4" s="115"/>
+      <c r="AH4" s="115"/>
       <c r="AI4" s="14" t="s">
         <v>50</v>
       </c>
@@ -4948,10 +4981,10 @@
       <c r="CB4" s="39" t="s">
         <v>189</v>
       </c>
-      <c r="CC4" s="119"/>
-      <c r="CD4" s="119"/>
-      <c r="CE4" s="119"/>
-      <c r="CF4" s="119"/>
+      <c r="CC4" s="105"/>
+      <c r="CD4" s="105"/>
+      <c r="CE4" s="105"/>
+      <c r="CF4" s="105"/>
       <c r="CG4" s="3" t="s">
         <v>20</v>
       </c>
@@ -6028,22 +6061,22 @@
     <row r="16" spans="1:90" s="44" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="CF3:CF4"/>
-    <mergeCell ref="CC3:CC4"/>
-    <mergeCell ref="CD3:CD4"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="M2:AD2"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AH3:AH4"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="AG3:AG4"/>
+    <mergeCell ref="AI2:BS2"/>
+    <mergeCell ref="BT2:CB2"/>
+    <mergeCell ref="CC2:CF2"/>
+    <mergeCell ref="CG2:CJ2"/>
+    <mergeCell ref="AY3:BA3"/>
+    <mergeCell ref="BB3:BK3"/>
+    <mergeCell ref="BQ3:BS3"/>
+    <mergeCell ref="BT3:BU3"/>
+    <mergeCell ref="BV3:BX3"/>
+    <mergeCell ref="BY3:CA3"/>
+    <mergeCell ref="BL3:BP3"/>
+    <mergeCell ref="AR3:AT3"/>
+    <mergeCell ref="AI3:AM3"/>
+    <mergeCell ref="AV3:AX3"/>
+    <mergeCell ref="AN3:AQ3"/>
+    <mergeCell ref="CE3:CE4"/>
     <mergeCell ref="B1:CL1"/>
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="R3:R4"/>
@@ -6060,22 +6093,22 @@
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
-    <mergeCell ref="AI2:BS2"/>
-    <mergeCell ref="BT2:CB2"/>
-    <mergeCell ref="CC2:CF2"/>
-    <mergeCell ref="CG2:CJ2"/>
-    <mergeCell ref="AY3:BA3"/>
-    <mergeCell ref="BB3:BK3"/>
-    <mergeCell ref="BQ3:BS3"/>
-    <mergeCell ref="BT3:BU3"/>
-    <mergeCell ref="BV3:BX3"/>
-    <mergeCell ref="BY3:CA3"/>
-    <mergeCell ref="BL3:BP3"/>
-    <mergeCell ref="AR3:AT3"/>
-    <mergeCell ref="AI3:AM3"/>
-    <mergeCell ref="AV3:AX3"/>
-    <mergeCell ref="AN3:AQ3"/>
-    <mergeCell ref="CE3:CE4"/>
+    <mergeCell ref="M2:AD2"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AH3:AH4"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="AF3:AF4"/>
+    <mergeCell ref="AG3:AG4"/>
+    <mergeCell ref="CF3:CF4"/>
+    <mergeCell ref="CC3:CC4"/>
+    <mergeCell ref="CD3:CD4"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="N3:O3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="CC8" r:id="rId1"/>
@@ -6090,8 +6123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CH45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView tabSelected="1" topLeftCell="BD1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6130,10 +6163,10 @@
         <v>553</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>104</v>
+        <v>555</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>37</v>
+        <v>556</v>
       </c>
       <c r="E1" s="51" t="s">
         <v>554</v>
@@ -6145,10 +6178,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="51" t="s">
-        <v>38</v>
+        <v>557</v>
       </c>
       <c r="I1" s="51" t="s">
-        <v>39</v>
+        <v>558</v>
       </c>
       <c r="J1" s="51" t="s">
         <v>7</v>
@@ -6157,19 +6190,19 @@
         <v>8</v>
       </c>
       <c r="L1" s="51" t="s">
-        <v>225</v>
+        <v>559</v>
       </c>
       <c r="M1" s="51" t="s">
-        <v>224</v>
+        <v>560</v>
       </c>
       <c r="N1" s="51" t="s">
-        <v>555</v>
+        <v>561</v>
       </c>
       <c r="O1" s="51" t="s">
-        <v>54</v>
+        <v>562</v>
       </c>
       <c r="P1" s="51" t="s">
-        <v>55</v>
+        <v>563</v>
       </c>
       <c r="Q1" s="51" t="s">
         <v>9</v>
@@ -6181,13 +6214,13 @@
         <v>227</v>
       </c>
       <c r="T1" s="51" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="U1" s="51" t="s">
-        <v>557</v>
+        <v>565</v>
       </c>
       <c r="V1" s="51" t="s">
-        <v>230</v>
+        <v>566</v>
       </c>
       <c r="W1" s="51" t="s">
         <v>10</v>
@@ -6203,10 +6236,10 @@
         <v>231</v>
       </c>
       <c r="AB1" s="51" t="s">
-        <v>232</v>
+        <v>567</v>
       </c>
       <c r="AC1" s="51" t="s">
-        <v>233</v>
+        <v>568</v>
       </c>
       <c r="AD1" s="51" t="s">
         <v>294</v>

</xml_diff>

<commit_message>
Match DB and Python - vessel names
</commit_message>
<xml_diff>
--- a/src/databases/Vessel_Database_python.xlsx
+++ b/src/databases/Vessel_Database_python.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Vessels DB - Intro" sheetId="18" r:id="rId1"/>
@@ -856,7 +856,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="568">
   <si>
     <t>Source of information</t>
   </si>
@@ -1986,9 +1986,6 @@
     <t>Cable Lay Barge</t>
   </si>
   <si>
-    <t>Cable Barge</t>
-  </si>
-  <si>
     <t>BV I✠</t>
   </si>
   <si>
@@ -2028,9 +2025,6 @@
     <t>Crane barge</t>
   </si>
   <si>
-    <t>Jack-up barg</t>
-  </si>
-  <si>
     <t>DNV ✠1A1 Crane Barge, DYnPoS-aUt, Wind Turbine  Service and Crane Unit, R2.</t>
   </si>
   <si>
@@ -2103,9 +2097,6 @@
     <t>Seven Borealis</t>
   </si>
   <si>
-    <t xml:space="preserve">Crane Vessel  </t>
-  </si>
-  <si>
     <t>DNV 1A1 Crane Vessel HELDK-SH OPP-F E0 DYNPOS-AUTRO NAUT-AW CLEAN DESIGN DK(+) BIS</t>
   </si>
   <si>
@@ -2157,9 +2148,6 @@
     <t>Nexans Skagerrak</t>
   </si>
   <si>
-    <t>Cable Vessel</t>
-  </si>
-  <si>
     <t>DNV ✠ 1A1 Cable Laying Vessel E0 DYNPOS-AUTR SILENT-E</t>
   </si>
   <si>
@@ -2265,9 +2253,6 @@
     <t>Penrhos Bay</t>
   </si>
   <si>
-    <t>WFSV</t>
-  </si>
-  <si>
     <t>DNV✠1A1 R2 LC Crew UK MCA Cat 2</t>
   </si>
   <si>
@@ -2686,6 +2671,18 @@
   </si>
   <si>
     <t>Heli tonnage</t>
+  </si>
+  <si>
+    <t>Tugboat</t>
+  </si>
+  <si>
+    <t>CLV</t>
+  </si>
+  <si>
+    <t>CTV</t>
+  </si>
+  <si>
+    <t>JUP Barge</t>
   </si>
 </sst>
 </file>
@@ -3214,7 +3211,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
@@ -3470,32 +3467,74 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
@@ -3503,125 +3542,86 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3934,86 +3934,86 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.453125" customWidth="1"/>
-    <col min="3" max="3" width="43.81640625" customWidth="1"/>
-    <col min="4" max="4" width="54.26953125" customWidth="1"/>
-    <col min="6" max="6" width="19.453125" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" customWidth="1"/>
+    <col min="4" max="4" width="54.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B2" s="34" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="101" t="s">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="95" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="95"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="101"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="101"/>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="101"/>
-      <c r="C6" s="101"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="101"/>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="95"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B7" s="101"/>
-      <c r="C7" s="101"/>
-      <c r="D7" s="101"/>
-      <c r="E7" s="101"/>
-      <c r="F7" s="101"/>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="95"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="95"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="101"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="101"/>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="95"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="95"/>
+      <c r="E8" s="95"/>
+      <c r="F8" s="95"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="101"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="95"/>
+      <c r="C9" s="95"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="95"/>
+      <c r="F9" s="95"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="33"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="2:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="102" t="s">
+    <row r="12" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="96" t="s">
         <v>175</v>
       </c>
-      <c r="C13" s="103"/>
+      <c r="C13" s="97"/>
       <c r="D13" s="32"/>
     </row>
-    <row r="14" spans="2:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="31" t="s">
         <v>174</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="29" t="s">
         <v>171</v>
       </c>
@@ -4035,7 +4035,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="29" t="s">
         <v>168</v>
       </c>
@@ -4046,136 +4046,136 @@
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="95" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="98" t="s">
         <v>165</v>
       </c>
-      <c r="C17" s="97" t="s">
+      <c r="C17" s="101" t="s">
         <v>164</v>
       </c>
       <c r="D17" s="22" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="99"/>
-      <c r="C18" s="100"/>
+      <c r="C18" s="102"/>
       <c r="D18" s="22" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="96"/>
-      <c r="C19" s="98"/>
+    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="100"/>
+      <c r="C19" s="103"/>
       <c r="D19" s="23" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="95" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="98" t="s">
         <v>160</v>
       </c>
-      <c r="C20" s="97" t="s">
+      <c r="C20" s="101" t="s">
         <v>159</v>
       </c>
       <c r="D20" s="22" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="96"/>
-      <c r="C21" s="98"/>
+    <row r="21" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="100"/>
+      <c r="C21" s="103"/>
       <c r="D21" s="23" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B22" s="95" t="s">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="98" t="s">
         <v>156</v>
       </c>
-      <c r="C22" s="97" t="s">
+      <c r="C22" s="101" t="s">
         <v>155</v>
       </c>
       <c r="D22" s="22" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="96"/>
-      <c r="C23" s="98"/>
+    <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="100"/>
+      <c r="C23" s="103"/>
       <c r="D23" s="23" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B24" s="95" t="s">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="98" t="s">
         <v>152</v>
       </c>
-      <c r="C24" s="97" t="s">
+      <c r="C24" s="101" t="s">
         <v>151</v>
       </c>
       <c r="D24" s="22" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="99"/>
-      <c r="C25" s="100"/>
+      <c r="C25" s="102"/>
       <c r="D25" s="22" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="96"/>
-      <c r="C26" s="98"/>
+    <row r="26" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="100"/>
+      <c r="C26" s="103"/>
       <c r="D26" s="23" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="95" t="s">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="98" t="s">
         <v>147</v>
       </c>
-      <c r="C27" s="97" t="s">
+      <c r="C27" s="101" t="s">
         <v>146</v>
       </c>
       <c r="D27" s="28" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="96"/>
-      <c r="C28" s="98"/>
+    <row r="28" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="100"/>
+      <c r="C28" s="103"/>
       <c r="D28" s="27" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B29" s="95" t="s">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="98" t="s">
         <v>143</v>
       </c>
-      <c r="C29" s="97" t="s">
+      <c r="C29" s="101" t="s">
         <v>142</v>
       </c>
       <c r="D29" s="22" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="99"/>
-      <c r="C30" s="100"/>
+      <c r="C30" s="102"/>
       <c r="D30" s="22" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="96"/>
-      <c r="C31" s="98"/>
+    <row r="31" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="100"/>
+      <c r="C31" s="103"/>
       <c r="D31" s="23" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="26" t="s">
         <v>138</v>
       </c>
@@ -4186,136 +4186,136 @@
         <v>136</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="95" t="s">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="98" t="s">
         <v>135</v>
       </c>
-      <c r="C33" s="97" t="s">
+      <c r="C33" s="101" t="s">
         <v>134</v>
       </c>
       <c r="D33" s="24" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="99"/>
-      <c r="C34" s="100"/>
+      <c r="C34" s="102"/>
       <c r="D34" s="22" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="96"/>
-      <c r="C35" s="98"/>
+    <row r="35" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="100"/>
+      <c r="C35" s="103"/>
       <c r="D35" s="23" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B36" s="95" t="s">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="98" t="s">
         <v>130</v>
       </c>
-      <c r="C36" s="97" t="s">
+      <c r="C36" s="101" t="s">
         <v>129</v>
       </c>
       <c r="D36" s="22" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="96"/>
-      <c r="C37" s="98"/>
+    <row r="37" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="100"/>
+      <c r="C37" s="103"/>
       <c r="D37" s="23" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B38" s="95" t="s">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="98" t="s">
         <v>126</v>
       </c>
-      <c r="C38" s="97" t="s">
+      <c r="C38" s="101" t="s">
         <v>125</v>
       </c>
       <c r="D38" s="22" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="39" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="96"/>
-      <c r="C39" s="98"/>
+    <row r="39" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="100"/>
+      <c r="C39" s="103"/>
       <c r="D39" s="23" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B40" s="95" t="s">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="98" t="s">
         <v>122</v>
       </c>
-      <c r="C40" s="97" t="s">
+      <c r="C40" s="101" t="s">
         <v>121</v>
       </c>
       <c r="D40" s="22" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="96"/>
-      <c r="C41" s="98"/>
+    <row r="41" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="100"/>
+      <c r="C41" s="103"/>
       <c r="D41" s="23" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B42" s="95" t="s">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="98" t="s">
         <v>118</v>
       </c>
-      <c r="C42" s="97" t="s">
+      <c r="C42" s="101" t="s">
         <v>117</v>
       </c>
       <c r="D42" s="22" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="99"/>
-      <c r="C43" s="100"/>
+      <c r="C43" s="102"/>
       <c r="D43" s="22" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="96"/>
-      <c r="C44" s="98"/>
+    <row r="44" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="100"/>
+      <c r="C44" s="103"/>
       <c r="D44" s="23" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="2:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="95" t="s">
+    <row r="45" spans="2:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="98" t="s">
         <v>113</v>
       </c>
-      <c r="C45" s="97" t="s">
+      <c r="C45" s="101" t="s">
         <v>112</v>
       </c>
       <c r="D45" s="22" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="99"/>
-      <c r="C46" s="100"/>
+      <c r="C46" s="102"/>
       <c r="D46" s="22" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="96"/>
-      <c r="C47" s="98"/>
+    <row r="47" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="100"/>
+      <c r="C47" s="103"/>
       <c r="D47" s="21" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="2:4" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:4" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="20" t="s">
         <v>108</v>
       </c>
@@ -4326,29 +4326,11 @@
         <v>106</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B4:F9"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="B45:B47"/>
@@ -4357,6 +4339,24 @@
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="C42:C44"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="B4:F9"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4370,409 +4370,409 @@
       <selection activeCell="BK8" sqref="BK8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="7" max="7" width="14.7265625" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" customWidth="1"/>
-    <col min="10" max="10" width="8.26953125" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" customWidth="1"/>
     <col min="26" max="26" width="11" customWidth="1"/>
     <col min="27" max="27" width="12" customWidth="1"/>
-    <col min="28" max="29" width="10.54296875" customWidth="1"/>
-    <col min="30" max="30" width="9.81640625" customWidth="1"/>
-    <col min="31" max="31" width="12.54296875" customWidth="1"/>
-    <col min="32" max="32" width="9.1796875" customWidth="1"/>
-    <col min="37" max="37" width="11.54296875" customWidth="1"/>
-    <col min="44" max="44" width="10.7265625" customWidth="1"/>
-    <col min="45" max="45" width="10.26953125" customWidth="1"/>
+    <col min="28" max="29" width="10.5703125" customWidth="1"/>
+    <col min="30" max="30" width="9.85546875" customWidth="1"/>
+    <col min="31" max="31" width="12.5703125" customWidth="1"/>
+    <col min="32" max="32" width="9.140625" customWidth="1"/>
+    <col min="37" max="37" width="11.5703125" customWidth="1"/>
+    <col min="44" max="44" width="10.7109375" customWidth="1"/>
+    <col min="45" max="45" width="10.28515625" customWidth="1"/>
     <col min="47" max="47" width="11" customWidth="1"/>
     <col min="48" max="48" width="8" customWidth="1"/>
-    <col min="49" max="49" width="9.453125" customWidth="1"/>
-    <col min="50" max="50" width="10.54296875" customWidth="1"/>
+    <col min="49" max="49" width="9.42578125" customWidth="1"/>
+    <col min="50" max="50" width="10.5703125" customWidth="1"/>
     <col min="51" max="51" width="11" customWidth="1"/>
-    <col min="52" max="52" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="64" width="10.81640625" customWidth="1"/>
-    <col min="65" max="65" width="8.453125" customWidth="1"/>
-    <col min="66" max="66" width="7.81640625" customWidth="1"/>
-    <col min="67" max="67" width="10.81640625" customWidth="1"/>
+    <col min="52" max="52" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="64" width="10.85546875" customWidth="1"/>
+    <col min="65" max="65" width="8.42578125" customWidth="1"/>
+    <col min="66" max="66" width="7.85546875" customWidth="1"/>
+    <col min="67" max="67" width="10.85546875" customWidth="1"/>
     <col min="68" max="68" width="8" customWidth="1"/>
-    <col min="75" max="75" width="12.1796875" customWidth="1"/>
-    <col min="76" max="76" width="11.26953125" customWidth="1"/>
-    <col min="77" max="77" width="11.81640625" customWidth="1"/>
-    <col min="78" max="78" width="9.453125" customWidth="1"/>
-    <col min="79" max="79" width="11.453125" customWidth="1"/>
-    <col min="80" max="80" width="25.453125" customWidth="1"/>
+    <col min="75" max="75" width="12.140625" customWidth="1"/>
+    <col min="76" max="76" width="11.28515625" customWidth="1"/>
+    <col min="77" max="77" width="11.85546875" customWidth="1"/>
+    <col min="78" max="78" width="9.42578125" customWidth="1"/>
+    <col min="79" max="79" width="11.42578125" customWidth="1"/>
+    <col min="80" max="80" width="25.42578125" customWidth="1"/>
     <col min="81" max="81" width="27" customWidth="1"/>
-    <col min="83" max="83" width="14.54296875" customWidth="1"/>
-    <col min="84" max="84" width="8.453125" customWidth="1"/>
-    <col min="85" max="85" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="14.5703125" customWidth="1"/>
+    <col min="84" max="84" width="8.42578125" customWidth="1"/>
+    <col min="85" max="85" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:90" ht="33.5" x14ac:dyDescent="0.35">
-      <c r="B1" s="121" t="s">
+    <row r="1" spans="1:90" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="120" t="s">
         <v>177</v>
       </c>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121"/>
-      <c r="I1" s="121"/>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="121"/>
-      <c r="O1" s="121"/>
-      <c r="P1" s="121"/>
-      <c r="Q1" s="121"/>
-      <c r="R1" s="121"/>
-      <c r="S1" s="121"/>
-      <c r="T1" s="121"/>
-      <c r="U1" s="121"/>
-      <c r="V1" s="121"/>
-      <c r="W1" s="121"/>
-      <c r="X1" s="121"/>
-      <c r="Y1" s="121"/>
-      <c r="Z1" s="121"/>
-      <c r="AA1" s="121"/>
-      <c r="AB1" s="121"/>
-      <c r="AC1" s="121"/>
-      <c r="AD1" s="121"/>
-      <c r="AE1" s="121"/>
-      <c r="AF1" s="121"/>
-      <c r="AG1" s="121"/>
-      <c r="AH1" s="121"/>
-      <c r="AI1" s="121"/>
-      <c r="AJ1" s="121"/>
-      <c r="AK1" s="121"/>
-      <c r="AL1" s="121"/>
-      <c r="AM1" s="121"/>
-      <c r="AN1" s="121"/>
-      <c r="AO1" s="121"/>
-      <c r="AP1" s="121"/>
-      <c r="AQ1" s="121"/>
-      <c r="AR1" s="121"/>
-      <c r="AS1" s="121"/>
-      <c r="AT1" s="121"/>
-      <c r="AU1" s="121"/>
-      <c r="AV1" s="121"/>
-      <c r="AW1" s="121"/>
-      <c r="AX1" s="121"/>
-      <c r="AY1" s="121"/>
-      <c r="AZ1" s="121"/>
-      <c r="BA1" s="121"/>
-      <c r="BB1" s="121"/>
-      <c r="BC1" s="121"/>
-      <c r="BD1" s="121"/>
-      <c r="BE1" s="121"/>
-      <c r="BF1" s="121"/>
-      <c r="BG1" s="121"/>
-      <c r="BH1" s="121"/>
-      <c r="BI1" s="121"/>
-      <c r="BJ1" s="121"/>
-      <c r="BK1" s="121"/>
-      <c r="BL1" s="121"/>
-      <c r="BM1" s="121"/>
-      <c r="BN1" s="121"/>
-      <c r="BO1" s="121"/>
-      <c r="BP1" s="121"/>
-      <c r="BQ1" s="121"/>
-      <c r="BR1" s="121"/>
-      <c r="BS1" s="121"/>
-      <c r="BT1" s="121"/>
-      <c r="BU1" s="121"/>
-      <c r="BV1" s="121"/>
-      <c r="BW1" s="121"/>
-      <c r="BX1" s="121"/>
-      <c r="BY1" s="121"/>
-      <c r="BZ1" s="121"/>
-      <c r="CA1" s="121"/>
-      <c r="CB1" s="121"/>
-      <c r="CC1" s="121"/>
-      <c r="CD1" s="121"/>
-      <c r="CE1" s="121"/>
-      <c r="CF1" s="121"/>
-      <c r="CG1" s="121"/>
-      <c r="CH1" s="121"/>
-      <c r="CI1" s="121"/>
-      <c r="CJ1" s="121"/>
-      <c r="CK1" s="121"/>
-      <c r="CL1" s="121"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="120"/>
+      <c r="O1" s="120"/>
+      <c r="P1" s="120"/>
+      <c r="Q1" s="120"/>
+      <c r="R1" s="120"/>
+      <c r="S1" s="120"/>
+      <c r="T1" s="120"/>
+      <c r="U1" s="120"/>
+      <c r="V1" s="120"/>
+      <c r="W1" s="120"/>
+      <c r="X1" s="120"/>
+      <c r="Y1" s="120"/>
+      <c r="Z1" s="120"/>
+      <c r="AA1" s="120"/>
+      <c r="AB1" s="120"/>
+      <c r="AC1" s="120"/>
+      <c r="AD1" s="120"/>
+      <c r="AE1" s="120"/>
+      <c r="AF1" s="120"/>
+      <c r="AG1" s="120"/>
+      <c r="AH1" s="120"/>
+      <c r="AI1" s="120"/>
+      <c r="AJ1" s="120"/>
+      <c r="AK1" s="120"/>
+      <c r="AL1" s="120"/>
+      <c r="AM1" s="120"/>
+      <c r="AN1" s="120"/>
+      <c r="AO1" s="120"/>
+      <c r="AP1" s="120"/>
+      <c r="AQ1" s="120"/>
+      <c r="AR1" s="120"/>
+      <c r="AS1" s="120"/>
+      <c r="AT1" s="120"/>
+      <c r="AU1" s="120"/>
+      <c r="AV1" s="120"/>
+      <c r="AW1" s="120"/>
+      <c r="AX1" s="120"/>
+      <c r="AY1" s="120"/>
+      <c r="AZ1" s="120"/>
+      <c r="BA1" s="120"/>
+      <c r="BB1" s="120"/>
+      <c r="BC1" s="120"/>
+      <c r="BD1" s="120"/>
+      <c r="BE1" s="120"/>
+      <c r="BF1" s="120"/>
+      <c r="BG1" s="120"/>
+      <c r="BH1" s="120"/>
+      <c r="BI1" s="120"/>
+      <c r="BJ1" s="120"/>
+      <c r="BK1" s="120"/>
+      <c r="BL1" s="120"/>
+      <c r="BM1" s="120"/>
+      <c r="BN1" s="120"/>
+      <c r="BO1" s="120"/>
+      <c r="BP1" s="120"/>
+      <c r="BQ1" s="120"/>
+      <c r="BR1" s="120"/>
+      <c r="BS1" s="120"/>
+      <c r="BT1" s="120"/>
+      <c r="BU1" s="120"/>
+      <c r="BV1" s="120"/>
+      <c r="BW1" s="120"/>
+      <c r="BX1" s="120"/>
+      <c r="BY1" s="120"/>
+      <c r="BZ1" s="120"/>
+      <c r="CA1" s="120"/>
+      <c r="CB1" s="120"/>
+      <c r="CC1" s="120"/>
+      <c r="CD1" s="120"/>
+      <c r="CE1" s="120"/>
+      <c r="CF1" s="120"/>
+      <c r="CG1" s="120"/>
+      <c r="CH1" s="120"/>
+      <c r="CI1" s="120"/>
+      <c r="CJ1" s="120"/>
+      <c r="CK1" s="120"/>
+      <c r="CL1" s="120"/>
     </row>
-    <row r="2" spans="1:90" s="42" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:90" s="42" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="43"/>
-      <c r="C2" s="122" t="s">
+      <c r="C2" s="123" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="123"/>
-      <c r="J2" s="123"/>
-      <c r="K2" s="123"/>
-      <c r="L2" s="124"/>
-      <c r="M2" s="109" t="s">
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="124"/>
+      <c r="J2" s="124"/>
+      <c r="K2" s="124"/>
+      <c r="L2" s="125"/>
+      <c r="M2" s="132" t="s">
         <v>65</v>
       </c>
-      <c r="N2" s="110"/>
-      <c r="O2" s="110"/>
-      <c r="P2" s="110"/>
-      <c r="Q2" s="110"/>
-      <c r="R2" s="110"/>
-      <c r="S2" s="110"/>
-      <c r="T2" s="110"/>
-      <c r="U2" s="110"/>
-      <c r="V2" s="110"/>
-      <c r="W2" s="110"/>
-      <c r="X2" s="110"/>
-      <c r="Y2" s="110"/>
-      <c r="Z2" s="110"/>
-      <c r="AA2" s="110"/>
-      <c r="AB2" s="110"/>
-      <c r="AC2" s="110"/>
-      <c r="AD2" s="111"/>
-      <c r="AE2" s="125" t="s">
+      <c r="N2" s="133"/>
+      <c r="O2" s="133"/>
+      <c r="P2" s="133"/>
+      <c r="Q2" s="133"/>
+      <c r="R2" s="133"/>
+      <c r="S2" s="133"/>
+      <c r="T2" s="133"/>
+      <c r="U2" s="133"/>
+      <c r="V2" s="133"/>
+      <c r="W2" s="133"/>
+      <c r="X2" s="133"/>
+      <c r="Y2" s="133"/>
+      <c r="Z2" s="133"/>
+      <c r="AA2" s="133"/>
+      <c r="AB2" s="133"/>
+      <c r="AC2" s="133"/>
+      <c r="AD2" s="134"/>
+      <c r="AE2" s="126" t="s">
         <v>178</v>
       </c>
-      <c r="AF2" s="125"/>
-      <c r="AG2" s="125"/>
-      <c r="AH2" s="125"/>
-      <c r="AI2" s="131" t="s">
+      <c r="AF2" s="126"/>
+      <c r="AG2" s="126"/>
+      <c r="AH2" s="126"/>
+      <c r="AI2" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="AJ2" s="132"/>
-      <c r="AK2" s="132"/>
-      <c r="AL2" s="132"/>
-      <c r="AM2" s="132"/>
-      <c r="AN2" s="132"/>
-      <c r="AO2" s="132"/>
-      <c r="AP2" s="132"/>
-      <c r="AQ2" s="132"/>
-      <c r="AR2" s="132"/>
-      <c r="AS2" s="132"/>
-      <c r="AT2" s="132"/>
-      <c r="AU2" s="132"/>
-      <c r="AV2" s="132"/>
-      <c r="AW2" s="132"/>
-      <c r="AX2" s="132"/>
-      <c r="AY2" s="132"/>
-      <c r="AZ2" s="132"/>
-      <c r="BA2" s="132"/>
-      <c r="BB2" s="132"/>
-      <c r="BC2" s="132"/>
-      <c r="BD2" s="132"/>
-      <c r="BE2" s="132"/>
-      <c r="BF2" s="132"/>
-      <c r="BG2" s="132"/>
-      <c r="BH2" s="132"/>
-      <c r="BI2" s="132"/>
-      <c r="BJ2" s="132"/>
-      <c r="BK2" s="132"/>
-      <c r="BL2" s="132"/>
-      <c r="BM2" s="132"/>
-      <c r="BN2" s="132"/>
-      <c r="BO2" s="132"/>
-      <c r="BP2" s="132"/>
-      <c r="BQ2" s="132"/>
-      <c r="BR2" s="132"/>
-      <c r="BS2" s="132"/>
-      <c r="BT2" s="133" t="s">
+      <c r="AJ2" s="105"/>
+      <c r="AK2" s="105"/>
+      <c r="AL2" s="105"/>
+      <c r="AM2" s="105"/>
+      <c r="AN2" s="105"/>
+      <c r="AO2" s="105"/>
+      <c r="AP2" s="105"/>
+      <c r="AQ2" s="105"/>
+      <c r="AR2" s="105"/>
+      <c r="AS2" s="105"/>
+      <c r="AT2" s="105"/>
+      <c r="AU2" s="105"/>
+      <c r="AV2" s="105"/>
+      <c r="AW2" s="105"/>
+      <c r="AX2" s="105"/>
+      <c r="AY2" s="105"/>
+      <c r="AZ2" s="105"/>
+      <c r="BA2" s="105"/>
+      <c r="BB2" s="105"/>
+      <c r="BC2" s="105"/>
+      <c r="BD2" s="105"/>
+      <c r="BE2" s="105"/>
+      <c r="BF2" s="105"/>
+      <c r="BG2" s="105"/>
+      <c r="BH2" s="105"/>
+      <c r="BI2" s="105"/>
+      <c r="BJ2" s="105"/>
+      <c r="BK2" s="105"/>
+      <c r="BL2" s="105"/>
+      <c r="BM2" s="105"/>
+      <c r="BN2" s="105"/>
+      <c r="BO2" s="105"/>
+      <c r="BP2" s="105"/>
+      <c r="BQ2" s="105"/>
+      <c r="BR2" s="105"/>
+      <c r="BS2" s="105"/>
+      <c r="BT2" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="BU2" s="133"/>
-      <c r="BV2" s="133"/>
-      <c r="BW2" s="133"/>
-      <c r="BX2" s="133"/>
-      <c r="BY2" s="133"/>
-      <c r="BZ2" s="133"/>
-      <c r="CA2" s="133"/>
-      <c r="CB2" s="133"/>
-      <c r="CC2" s="134" t="s">
+      <c r="BU2" s="106"/>
+      <c r="BV2" s="106"/>
+      <c r="BW2" s="106"/>
+      <c r="BX2" s="106"/>
+      <c r="BY2" s="106"/>
+      <c r="BZ2" s="106"/>
+      <c r="CA2" s="106"/>
+      <c r="CB2" s="106"/>
+      <c r="CC2" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="CD2" s="134"/>
-      <c r="CE2" s="134"/>
-      <c r="CF2" s="134"/>
-      <c r="CG2" s="135" t="s">
+      <c r="CD2" s="107"/>
+      <c r="CE2" s="107"/>
+      <c r="CF2" s="107"/>
+      <c r="CG2" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="CH2" s="135"/>
-      <c r="CI2" s="135"/>
-      <c r="CJ2" s="135"/>
+      <c r="CH2" s="108"/>
+      <c r="CI2" s="108"/>
+      <c r="CJ2" s="108"/>
     </row>
-    <row r="3" spans="1:90" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="127" t="s">
+    <row r="3" spans="1:90" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="126" t="s">
+      <c r="C3" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="128" t="s">
+      <c r="D3" s="129" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="126" t="s">
+      <c r="E3" s="127" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="126" t="s">
+      <c r="F3" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="126" t="s">
+      <c r="G3" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="130" t="s">
+      <c r="H3" s="131" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="126" t="s">
+      <c r="I3" s="127" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="126" t="s">
+      <c r="J3" s="127" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="126" t="s">
+      <c r="K3" s="127" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="126" t="s">
+      <c r="L3" s="127" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="118" t="s">
+      <c r="M3" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="N3" s="108" t="s">
+      <c r="N3" s="141" t="s">
         <v>57</v>
       </c>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108" t="s">
+      <c r="O3" s="141"/>
+      <c r="P3" s="141" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="118" t="s">
+      <c r="Q3" s="141"/>
+      <c r="R3" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="118" t="s">
+      <c r="S3" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="T3" s="118" t="s">
+      <c r="T3" s="121" t="s">
         <v>13</v>
       </c>
-      <c r="U3" s="116" t="s">
+      <c r="U3" s="139" t="s">
         <v>66</v>
       </c>
-      <c r="V3" s="117"/>
-      <c r="W3" s="120"/>
-      <c r="X3" s="116" t="s">
+      <c r="V3" s="140"/>
+      <c r="W3" s="142"/>
+      <c r="X3" s="139" t="s">
         <v>53</v>
       </c>
-      <c r="Y3" s="117"/>
+      <c r="Y3" s="140"/>
       <c r="Z3" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="AA3" s="106" t="s">
+      <c r="AA3" s="143" t="s">
         <v>98</v>
       </c>
-      <c r="AB3" s="107"/>
-      <c r="AC3" s="112" t="s">
+      <c r="AB3" s="144"/>
+      <c r="AC3" s="135" t="s">
         <v>48</v>
       </c>
-      <c r="AD3" s="113"/>
-      <c r="AE3" s="114" t="s">
+      <c r="AD3" s="136"/>
+      <c r="AE3" s="137" t="s">
         <v>47</v>
       </c>
-      <c r="AF3" s="114" t="s">
+      <c r="AF3" s="137" t="s">
         <v>201</v>
       </c>
-      <c r="AG3" s="114" t="s">
+      <c r="AG3" s="137" t="s">
         <v>202</v>
       </c>
-      <c r="AH3" s="114" t="s">
+      <c r="AH3" s="137" t="s">
         <v>203</v>
       </c>
-      <c r="AI3" s="142" t="s">
+      <c r="AI3" s="115" t="s">
         <v>63</v>
       </c>
-      <c r="AJ3" s="143"/>
-      <c r="AK3" s="143"/>
-      <c r="AL3" s="143"/>
-      <c r="AM3" s="144"/>
-      <c r="AN3" s="142" t="s">
+      <c r="AJ3" s="116"/>
+      <c r="AK3" s="116"/>
+      <c r="AL3" s="116"/>
+      <c r="AM3" s="117"/>
+      <c r="AN3" s="115" t="s">
         <v>60</v>
       </c>
-      <c r="AO3" s="143"/>
-      <c r="AP3" s="143"/>
-      <c r="AQ3" s="144"/>
-      <c r="AR3" s="142" t="s">
+      <c r="AO3" s="116"/>
+      <c r="AP3" s="116"/>
+      <c r="AQ3" s="117"/>
+      <c r="AR3" s="115" t="s">
         <v>73</v>
       </c>
-      <c r="AS3" s="143"/>
-      <c r="AT3" s="143"/>
+      <c r="AS3" s="116"/>
+      <c r="AT3" s="116"/>
       <c r="AU3" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="AV3" s="136" t="s">
+      <c r="AV3" s="109" t="s">
         <v>102</v>
       </c>
-      <c r="AW3" s="137"/>
-      <c r="AX3" s="138"/>
-      <c r="AY3" s="136" t="s">
+      <c r="AW3" s="110"/>
+      <c r="AX3" s="111"/>
+      <c r="AY3" s="109" t="s">
         <v>80</v>
       </c>
-      <c r="AZ3" s="137"/>
-      <c r="BA3" s="138"/>
-      <c r="BB3" s="136" t="s">
+      <c r="AZ3" s="110"/>
+      <c r="BA3" s="111"/>
+      <c r="BB3" s="109" t="s">
         <v>85</v>
       </c>
-      <c r="BC3" s="137"/>
-      <c r="BD3" s="137"/>
-      <c r="BE3" s="137"/>
-      <c r="BF3" s="137"/>
-      <c r="BG3" s="137"/>
-      <c r="BH3" s="137"/>
-      <c r="BI3" s="137"/>
-      <c r="BJ3" s="137"/>
-      <c r="BK3" s="138"/>
-      <c r="BL3" s="136" t="s">
+      <c r="BC3" s="110"/>
+      <c r="BD3" s="110"/>
+      <c r="BE3" s="110"/>
+      <c r="BF3" s="110"/>
+      <c r="BG3" s="110"/>
+      <c r="BH3" s="110"/>
+      <c r="BI3" s="110"/>
+      <c r="BJ3" s="110"/>
+      <c r="BK3" s="111"/>
+      <c r="BL3" s="109" t="s">
         <v>205</v>
       </c>
-      <c r="BM3" s="137"/>
-      <c r="BN3" s="137"/>
-      <c r="BO3" s="137"/>
-      <c r="BP3" s="137"/>
-      <c r="BQ3" s="136" t="s">
+      <c r="BM3" s="110"/>
+      <c r="BN3" s="110"/>
+      <c r="BO3" s="110"/>
+      <c r="BP3" s="110"/>
+      <c r="BQ3" s="109" t="s">
         <v>86</v>
       </c>
-      <c r="BR3" s="137"/>
-      <c r="BS3" s="137"/>
-      <c r="BT3" s="139" t="s">
+      <c r="BR3" s="110"/>
+      <c r="BS3" s="110"/>
+      <c r="BT3" s="112" t="s">
         <v>180</v>
       </c>
-      <c r="BU3" s="140"/>
-      <c r="BV3" s="139" t="s">
+      <c r="BU3" s="113"/>
+      <c r="BV3" s="112" t="s">
         <v>181</v>
       </c>
-      <c r="BW3" s="141"/>
-      <c r="BX3" s="141"/>
-      <c r="BY3" s="139" t="s">
+      <c r="BW3" s="114"/>
+      <c r="BX3" s="114"/>
+      <c r="BY3" s="112" t="s">
         <v>182</v>
       </c>
-      <c r="BZ3" s="141"/>
-      <c r="CA3" s="140"/>
+      <c r="BZ3" s="114"/>
+      <c r="CA3" s="113"/>
       <c r="CB3" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="CC3" s="104" t="s">
+      <c r="CC3" s="118" t="s">
         <v>16</v>
       </c>
-      <c r="CD3" s="104" t="s">
+      <c r="CD3" s="118" t="s">
         <v>17</v>
       </c>
-      <c r="CE3" s="104" t="s">
+      <c r="CE3" s="118" t="s">
         <v>18</v>
       </c>
-      <c r="CF3" s="104" t="s">
+      <c r="CF3" s="118" t="s">
         <v>19</v>
       </c>
       <c r="CG3" s="12"/>
@@ -4780,20 +4780,20 @@
       <c r="CI3" s="13"/>
       <c r="CJ3" s="13"/>
     </row>
-    <row r="4" spans="1:90" ht="134.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:90" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="127"/>
-      <c r="C4" s="126"/>
-      <c r="D4" s="129"/>
-      <c r="E4" s="126"/>
-      <c r="F4" s="126"/>
-      <c r="G4" s="126"/>
-      <c r="H4" s="130"/>
-      <c r="I4" s="126"/>
-      <c r="J4" s="126"/>
-      <c r="K4" s="126"/>
-      <c r="L4" s="126"/>
-      <c r="M4" s="119"/>
+      <c r="B4" s="128"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="130"/>
+      <c r="E4" s="127"/>
+      <c r="F4" s="127"/>
+      <c r="G4" s="127"/>
+      <c r="H4" s="131"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127"/>
+      <c r="L4" s="127"/>
+      <c r="M4" s="122"/>
       <c r="N4" s="2" t="s">
         <v>40</v>
       </c>
@@ -4806,9 +4806,9 @@
       <c r="Q4" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="R4" s="119"/>
-      <c r="S4" s="119"/>
-      <c r="T4" s="119"/>
+      <c r="R4" s="122"/>
+      <c r="S4" s="122"/>
+      <c r="T4" s="122"/>
       <c r="U4" s="2" t="s">
         <v>42</v>
       </c>
@@ -4839,10 +4839,10 @@
       <c r="AD4" s="35" t="s">
         <v>216</v>
       </c>
-      <c r="AE4" s="115"/>
-      <c r="AF4" s="115"/>
-      <c r="AG4" s="115"/>
-      <c r="AH4" s="115"/>
+      <c r="AE4" s="138"/>
+      <c r="AF4" s="138"/>
+      <c r="AG4" s="138"/>
+      <c r="AH4" s="138"/>
       <c r="AI4" s="14" t="s">
         <v>50</v>
       </c>
@@ -4981,10 +4981,10 @@
       <c r="CB4" s="39" t="s">
         <v>189</v>
       </c>
-      <c r="CC4" s="105"/>
-      <c r="CD4" s="105"/>
-      <c r="CE4" s="105"/>
-      <c r="CF4" s="105"/>
+      <c r="CC4" s="119"/>
+      <c r="CD4" s="119"/>
+      <c r="CE4" s="119"/>
+      <c r="CF4" s="119"/>
       <c r="CG4" s="3" t="s">
         <v>20</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:90" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:90" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>24</v>
       </c>
@@ -5262,7 +5262,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:90" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:90" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>36</v>
       </c>
@@ -5528,7 +5528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:90" s="49" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:90" s="49" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="50"/>
       <c r="C7" s="51" t="s">
         <v>3</v>
@@ -5755,7 +5755,7 @@
       <c r="CI7" s="51"/>
       <c r="CJ7" s="51"/>
     </row>
-    <row r="8" spans="1:90" s="44" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:90" s="44" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="45" t="s">
         <v>191</v>
       </c>
@@ -5899,7 +5899,7 @@
       <c r="CG8" s="45"/>
       <c r="CH8" s="45"/>
     </row>
-    <row r="9" spans="1:90" s="44" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:90" s="44" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="C9" s="44" t="s">
         <v>211</v>
       </c>
@@ -6006,7 +6006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:90" s="44" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:90" s="44" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="44" t="s">
         <v>219</v>
       </c>
@@ -6053,14 +6053,46 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:90" s="44" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:90" s="44" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:90" s="44" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:90" s="44" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:90" s="44" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:90" s="44" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:90" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:90" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:90" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:90" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:90" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:90" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="CF3:CF4"/>
+    <mergeCell ref="CC3:CC4"/>
+    <mergeCell ref="CD3:CD4"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="M2:AD2"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AH3:AH4"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="AF3:AF4"/>
+    <mergeCell ref="AG3:AG4"/>
+    <mergeCell ref="B1:CL1"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
     <mergeCell ref="AI2:BS2"/>
     <mergeCell ref="BT2:CB2"/>
     <mergeCell ref="CC2:CF2"/>
@@ -6077,38 +6109,6 @@
     <mergeCell ref="AV3:AX3"/>
     <mergeCell ref="AN3:AQ3"/>
     <mergeCell ref="CE3:CE4"/>
-    <mergeCell ref="B1:CL1"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="M2:AD2"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AH3:AH4"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="AG3:AG4"/>
-    <mergeCell ref="CF3:CF4"/>
-    <mergeCell ref="CC3:CC4"/>
-    <mergeCell ref="CD3:CD4"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="N3:O3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="CC8" r:id="rId1"/>
@@ -6123,53 +6123,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CH45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BD1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.1796875" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="16.453125" customWidth="1"/>
-    <col min="19" max="19" width="15.26953125" customWidth="1"/>
-    <col min="27" max="27" width="15.54296875" customWidth="1"/>
-    <col min="28" max="28" width="12.54296875" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" customWidth="1"/>
+    <col min="19" max="19" width="15.28515625" customWidth="1"/>
+    <col min="27" max="27" width="15.5703125" customWidth="1"/>
+    <col min="28" max="28" width="12.5703125" customWidth="1"/>
     <col min="29" max="29" width="13" customWidth="1"/>
-    <col min="32" max="32" width="10.81640625" customWidth="1"/>
-    <col min="36" max="36" width="10.81640625" customWidth="1"/>
-    <col min="38" max="38" width="10.453125" customWidth="1"/>
-    <col min="43" max="43" width="10.7265625" customWidth="1"/>
-    <col min="44" max="44" width="13.1796875" customWidth="1"/>
-    <col min="45" max="45" width="11.54296875" customWidth="1"/>
-    <col min="46" max="46" width="11.7265625" customWidth="1"/>
+    <col min="32" max="32" width="10.85546875" customWidth="1"/>
+    <col min="36" max="36" width="10.85546875" customWidth="1"/>
+    <col min="38" max="38" width="10.42578125" customWidth="1"/>
+    <col min="43" max="43" width="10.7109375" customWidth="1"/>
+    <col min="44" max="44" width="13.140625" customWidth="1"/>
+    <col min="45" max="45" width="11.5703125" customWidth="1"/>
+    <col min="46" max="46" width="11.7109375" customWidth="1"/>
     <col min="47" max="47" width="12" customWidth="1"/>
-    <col min="48" max="48" width="14.453125" customWidth="1"/>
+    <col min="48" max="48" width="14.42578125" customWidth="1"/>
     <col min="49" max="49" width="14" customWidth="1"/>
-    <col min="51" max="51" width="13.54296875" customWidth="1"/>
-    <col min="54" max="55" width="12.7265625" customWidth="1"/>
-    <col min="56" max="56" width="11.26953125" customWidth="1"/>
-    <col min="59" max="59" width="11.7265625" customWidth="1"/>
-    <col min="64" max="64" width="12.81640625" customWidth="1"/>
+    <col min="51" max="51" width="13.5703125" customWidth="1"/>
+    <col min="54" max="55" width="12.7109375" customWidth="1"/>
+    <col min="56" max="56" width="11.28515625" customWidth="1"/>
+    <col min="59" max="59" width="11.7109375" customWidth="1"/>
+    <col min="64" max="64" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:86" s="49" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:86" s="49" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="51" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="E1" s="51" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="F1" s="51" t="s">
         <v>5</v>
@@ -6178,10 +6179,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="51" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="I1" s="51" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="J1" s="51" t="s">
         <v>7</v>
@@ -6190,19 +6191,19 @@
         <v>8</v>
       </c>
       <c r="L1" s="51" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="M1" s="51" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="N1" s="51" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="O1" s="51" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="P1" s="51" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="Q1" s="51" t="s">
         <v>9</v>
@@ -6214,13 +6215,13 @@
         <v>227</v>
       </c>
       <c r="T1" s="51" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="U1" s="51" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="V1" s="51" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="W1" s="51" t="s">
         <v>10</v>
@@ -6236,10 +6237,10 @@
         <v>231</v>
       </c>
       <c r="AB1" s="51" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="AC1" s="51" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="AD1" s="51" t="s">
         <v>294</v>
@@ -6391,7 +6392,7 @@
       <c r="CG1" s="51"/>
       <c r="CH1" s="51"/>
     </row>
-    <row r="2" spans="1:86" s="44" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:86" s="44" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -6549,7 +6550,7 @@
       <c r="CE2" s="45"/>
       <c r="CF2" s="45"/>
     </row>
-    <row r="3" spans="1:86" s="44" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:86" s="44" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -6703,7 +6704,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="4" spans="1:86" s="44" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:86" s="44" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="65">
         <v>2</v>
       </c>
@@ -6714,13 +6715,13 @@
         <v>334</v>
       </c>
       <c r="D4" s="66" t="s">
+        <v>546</v>
+      </c>
+      <c r="E4" s="65" t="s">
         <v>335</v>
       </c>
-      <c r="E4" s="65" t="s">
+      <c r="F4" s="66" t="s">
         <v>336</v>
-      </c>
-      <c r="F4" s="66" t="s">
-        <v>337</v>
       </c>
       <c r="G4" s="68">
         <v>1977</v>
@@ -6732,7 +6733,7 @@
         <v>330</v>
       </c>
       <c r="J4" s="67" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K4" s="66">
         <v>2172</v>
@@ -6794,7 +6795,7 @@
       <c r="AN4" s="70"/>
       <c r="AO4" s="70"/>
       <c r="AP4" s="145" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AQ4" s="145"/>
       <c r="AR4" s="145"/>
@@ -6855,24 +6856,24 @@
         <v>132000</v>
       </c>
     </row>
-    <row r="5" spans="1:86" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:86" ht="120" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C5" s="53" t="s">
         <v>334</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>335</v>
+        <v>546</v>
       </c>
       <c r="E5" s="49" t="s">
+        <v>340</v>
+      </c>
+      <c r="F5" s="52" t="s">
         <v>341</v>
-      </c>
-      <c r="F5" s="52" t="s">
-        <v>342</v>
       </c>
       <c r="G5" s="55">
         <v>1970</v>
@@ -6884,7 +6885,7 @@
         <v>330</v>
       </c>
       <c r="J5" s="54" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K5">
         <v>2500</v>
@@ -6947,7 +6948,7 @@
       </c>
       <c r="AL5" s="65"/>
       <c r="AM5" s="54" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AN5" s="55" t="s">
         <v>322</v>
@@ -6981,13 +6982,13 @@
       <c r="AY5" s="60"/>
       <c r="AZ5" s="59"/>
       <c r="BA5" s="55" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="BB5" s="55">
         <v>0</v>
       </c>
       <c r="BC5" s="55" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="BD5" s="55">
         <v>2000</v>
@@ -7029,24 +7030,24 @@
         <v>132000</v>
       </c>
     </row>
-    <row r="6" spans="1:86" ht="87" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:86" ht="105" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" s="66" t="s">
+        <v>346</v>
+      </c>
+      <c r="C6" s="67" t="s">
         <v>347</v>
       </c>
-      <c r="C6" s="67" t="s">
+      <c r="D6" s="66" t="s">
+        <v>567</v>
+      </c>
+      <c r="E6" s="67" t="s">
         <v>348</v>
       </c>
-      <c r="D6" s="66" t="s">
+      <c r="F6" s="66" t="s">
         <v>349</v>
-      </c>
-      <c r="E6" s="67" t="s">
-        <v>350</v>
-      </c>
-      <c r="F6" s="66" t="s">
-        <v>351</v>
       </c>
       <c r="G6" s="68">
         <v>2010</v>
@@ -7055,10 +7056,10 @@
         <v>2013</v>
       </c>
       <c r="I6" s="68" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="J6" s="66" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="K6" s="66">
         <v>1989</v>
@@ -7131,7 +7132,7 @@
         <v>19</v>
       </c>
       <c r="AM6" s="66" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AN6" s="68" t="s">
         <v>322</v>
@@ -7197,12 +7198,12 @@
         <v>79000</v>
       </c>
     </row>
-    <row r="7" spans="1:86" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:86" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" s="65" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C7" s="67" t="s">
         <v>165</v>
@@ -7211,10 +7212,10 @@
         <v>165</v>
       </c>
       <c r="E7" s="67" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F7" s="67" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G7" s="68">
         <v>2002</v>
@@ -7226,7 +7227,7 @@
         <v>330</v>
       </c>
       <c r="J7" s="66" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="K7" s="65">
         <v>3898</v>
@@ -7285,7 +7286,7 @@
         <v>23</v>
       </c>
       <c r="AM7" s="66" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="AN7" s="68" t="s">
         <v>322</v>
@@ -7339,24 +7340,24 @@
         <v>29000</v>
       </c>
     </row>
-    <row r="8" spans="1:86" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:86" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="65">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D8" s="53" t="s">
         <v>165</v>
       </c>
       <c r="E8" s="54" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F8" s="53" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G8" s="55">
         <v>2009</v>
@@ -7368,7 +7369,7 @@
         <v>330</v>
       </c>
       <c r="J8" s="53" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="K8">
         <v>10873</v>
@@ -7426,10 +7427,10 @@
         <v>1.5</v>
       </c>
       <c r="AD8" s="56" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="AE8" s="56" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="AF8" s="49">
         <v>12</v>
@@ -7442,7 +7443,7 @@
         <v>1500</v>
       </c>
       <c r="AM8" s="54" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="AN8" s="55" t="s">
         <v>322</v>
@@ -7496,24 +7497,24 @@
         <v>52000</v>
       </c>
     </row>
-    <row r="9" spans="1:86" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:86" ht="45" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" s="66" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C9" s="67" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D9" s="66" t="s">
         <v>165</v>
       </c>
       <c r="E9" s="67" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F9" s="67" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G9" s="68">
         <v>1976</v>
@@ -7522,10 +7523,10 @@
         <v>1996</v>
       </c>
       <c r="I9" s="68" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="J9" s="66" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="K9" s="66">
         <v>6846</v>
@@ -7584,13 +7585,13 @@
       </c>
       <c r="AL9" s="66"/>
       <c r="AM9" s="66" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="AN9" s="68" t="s">
         <v>322</v>
       </c>
       <c r="AO9" s="68" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="AP9" s="70"/>
       <c r="AQ9" s="70"/>
@@ -7638,24 +7639,24 @@
         <v>420000</v>
       </c>
     </row>
-    <row r="10" spans="1:86" ht="122" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:86" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" s="66" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C10" s="67" t="s">
         <v>160</v>
       </c>
       <c r="D10" s="66" t="s">
-        <v>374</v>
+        <v>160</v>
       </c>
       <c r="E10" s="79" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="F10" s="66" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G10" s="68">
         <v>2012</v>
@@ -7664,10 +7665,10 @@
         <v>322</v>
       </c>
       <c r="I10" s="68" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="J10" s="66" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="K10" s="66">
         <v>49735</v>
@@ -7730,11 +7731,11 @@
         <v>40</v>
       </c>
       <c r="AM10" s="66" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="AN10" s="68"/>
       <c r="AO10" s="68" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="AP10" s="70"/>
       <c r="AQ10" s="70"/>
@@ -7782,12 +7783,12 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="11" spans="1:86" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" s="65" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C11" s="80" t="s">
         <v>165</v>
@@ -7796,10 +7797,10 @@
         <v>165</v>
       </c>
       <c r="E11" s="66" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="F11" s="80" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="G11" s="68">
         <v>1986</v>
@@ -7808,10 +7809,10 @@
         <v>2011</v>
       </c>
       <c r="I11" s="68" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="J11" s="66" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="K11" s="66">
         <v>1793</v>
@@ -7865,10 +7866,10 @@
         <v>1.5</v>
       </c>
       <c r="AD11" s="69" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="AE11" s="69" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="AF11" s="69" t="s">
         <v>322</v>
@@ -7936,24 +7937,24 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="12" spans="1:86" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:86" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="65">
         <v>10</v>
       </c>
       <c r="B12" s="65" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C12" s="80" t="s">
         <v>160</v>
       </c>
       <c r="D12" s="80" t="s">
-        <v>374</v>
+        <v>160</v>
       </c>
       <c r="E12" s="67" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F12" s="81" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="G12" s="68">
         <v>2011</v>
@@ -7962,10 +7963,10 @@
         <v>322</v>
       </c>
       <c r="I12" s="68" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="J12" s="67" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="K12" s="66">
         <v>15199</v>
@@ -8022,7 +8023,7 @@
         <v>16</v>
       </c>
       <c r="AM12" s="66" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AN12" s="68" t="s">
         <v>322</v>
@@ -8076,24 +8077,24 @@
         <v>419000</v>
       </c>
     </row>
-    <row r="13" spans="1:86" ht="81.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:86" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" s="66" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C13" s="80" t="s">
         <v>156</v>
       </c>
       <c r="D13" s="80" t="s">
-        <v>392</v>
+        <v>565</v>
       </c>
       <c r="E13" s="79" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="F13" s="81" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="G13" s="68">
         <v>1976</v>
@@ -8105,7 +8106,7 @@
         <v>323</v>
       </c>
       <c r="J13" s="66" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K13" s="66">
         <v>10147</v>
@@ -8185,7 +8186,7 @@
         <v>322</v>
       </c>
       <c r="AV13" s="68" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="AW13" s="68">
         <v>2</v>
@@ -8196,13 +8197,13 @@
       <c r="AY13" s="70"/>
       <c r="AZ13" s="70"/>
       <c r="BA13" s="68" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="BB13" s="68">
         <v>0</v>
       </c>
       <c r="BC13" s="68" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="BD13" s="68">
         <v>500</v>
@@ -8234,24 +8235,24 @@
         <v>174000</v>
       </c>
     </row>
-    <row r="14" spans="1:86" ht="116" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:86" ht="120" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" s="66" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C14" s="80" t="s">
         <v>156</v>
       </c>
       <c r="D14" s="80" t="s">
-        <v>392</v>
+        <v>565</v>
       </c>
       <c r="E14" s="67" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="F14" s="81" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="G14" s="68">
         <v>1999</v>
@@ -8260,10 +8261,10 @@
         <v>322</v>
       </c>
       <c r="I14" s="68" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="J14" s="66" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="K14" s="66">
         <v>4904</v>
@@ -8328,7 +8329,7 @@
         <v>26.5</v>
       </c>
       <c r="AM14" s="67" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="AN14" s="68" t="s">
         <v>322</v>
@@ -8364,13 +8365,13 @@
       <c r="AY14" s="70"/>
       <c r="AZ14" s="70"/>
       <c r="BA14" s="68" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="BB14" s="68">
         <v>0</v>
       </c>
       <c r="BC14" s="68" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="BD14" s="56">
         <v>0</v>
@@ -8394,7 +8395,7 @@
         <v>4</v>
       </c>
       <c r="BO14" s="67" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="BP14" s="70"/>
       <c r="BQ14" s="70"/>
@@ -8412,24 +8413,24 @@
         <v>132000</v>
       </c>
     </row>
-    <row r="15" spans="1:86" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:86" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" s="65" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C15" s="80" t="s">
         <v>156</v>
       </c>
       <c r="D15" s="80" t="s">
-        <v>392</v>
+        <v>565</v>
       </c>
       <c r="E15" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="F15" s="81" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="G15" s="68">
         <v>2010</v>
@@ -8438,10 +8439,10 @@
         <v>322</v>
       </c>
       <c r="I15" s="68" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="J15" s="82" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="K15" s="65">
         <v>2525</v>
@@ -8499,7 +8500,7 @@
         <v>1.5</v>
       </c>
       <c r="AD15" s="76" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="AE15" s="65">
         <v>2.5</v>
@@ -8518,7 +8519,7 @@
         <v>20</v>
       </c>
       <c r="AM15" s="67" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="AN15" s="68" t="s">
         <v>322</v>
@@ -8550,13 +8551,13 @@
       <c r="AY15" s="70"/>
       <c r="AZ15" s="70"/>
       <c r="BA15" s="68" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="BB15" s="55">
         <v>0</v>
       </c>
       <c r="BC15" s="68" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="BD15" s="68">
         <v>2500</v>
@@ -8592,24 +8593,24 @@
         <v>132000</v>
       </c>
     </row>
-    <row r="16" spans="1:86" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:86" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="65">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C16" s="53" t="s">
         <v>156</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>392</v>
+        <v>565</v>
       </c>
       <c r="E16" s="54" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="F16" s="52" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="G16" s="55">
         <v>1984</v>
@@ -8618,10 +8619,10 @@
         <v>322</v>
       </c>
       <c r="I16" s="55" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="J16" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="K16">
         <v>10674</v>
@@ -8692,7 +8693,7 @@
         <v>22</v>
       </c>
       <c r="AM16" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="AN16" s="55" t="s">
         <v>322</v>
@@ -8749,12 +8750,12 @@
         <v>130000</v>
       </c>
     </row>
-    <row r="17" spans="1:74" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:74" ht="75" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C17" s="53" t="s">
         <v>152</v>
@@ -8763,10 +8764,10 @@
         <v>319</v>
       </c>
       <c r="E17" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="F17" s="52" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="G17" s="55">
         <v>2007</v>
@@ -8775,10 +8776,10 @@
         <v>322</v>
       </c>
       <c r="I17" s="55" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="J17" s="54" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="K17">
         <v>4953</v>
@@ -8843,7 +8844,7 @@
         <v>25</v>
       </c>
       <c r="AM17" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="AO17" s="55" t="s">
         <v>327</v>
@@ -8904,24 +8905,24 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="18" spans="1:74" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:74" ht="30" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" s="66" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="C18" s="80" t="s">
         <v>152</v>
       </c>
       <c r="D18" s="80" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="E18" s="65" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="F18" s="80" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G18" s="68">
         <v>1973</v>
@@ -8930,10 +8931,10 @@
         <v>322</v>
       </c>
       <c r="I18" s="68" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="J18" s="66" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="K18" s="65">
         <v>125</v>
@@ -9046,24 +9047,24 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="19" spans="1:74" ht="58" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:74" ht="60" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C19" s="53" t="s">
         <v>152</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>428</v>
+        <v>566</v>
       </c>
       <c r="E19" s="57" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="F19" s="53" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="G19" s="55">
         <v>2010</v>
@@ -9072,10 +9073,10 @@
         <v>322</v>
       </c>
       <c r="I19" s="55" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="J19" s="54" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="K19">
         <v>70</v>
@@ -9152,7 +9153,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="AM19" s="54" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="AN19" s="55" t="s">
         <v>322</v>
@@ -9206,24 +9207,24 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="20" spans="1:74" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:74" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="65">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C20" s="53" t="s">
         <v>147</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="E20" s="84" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="F20" s="52" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G20" s="55">
         <v>1984</v>
@@ -9232,10 +9233,10 @@
         <v>2002</v>
       </c>
       <c r="I20" s="55" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="J20" s="54" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="K20">
         <v>6254</v>
@@ -9301,13 +9302,13 @@
         <v>10</v>
       </c>
       <c r="AM20" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="AN20">
         <v>2000</v>
       </c>
       <c r="AO20" s="55" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="AP20" s="59"/>
       <c r="AQ20" s="59"/>
@@ -9320,7 +9321,7 @@
         <v>3</v>
       </c>
       <c r="AX20" s="55" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="AY20">
         <v>450</v>
@@ -9329,13 +9330,13 @@
         <v>18</v>
       </c>
       <c r="BA20" s="55" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="BB20" s="55">
         <v>1600</v>
       </c>
       <c r="BC20" s="68" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="BD20" s="69">
         <v>0</v>
@@ -9367,24 +9368,24 @@
         <v>209000</v>
       </c>
     </row>
-    <row r="21" spans="1:74" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:74" ht="105" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" s="66" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="C21" s="80" t="s">
         <v>147</v>
       </c>
       <c r="D21" s="80" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="E21" s="85" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="F21" s="81" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="G21" s="68">
         <v>2011</v>
@@ -9393,10 +9394,10 @@
         <v>322</v>
       </c>
       <c r="I21" s="68" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="J21" s="66" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="K21" s="66">
         <v>7238</v>
@@ -9457,13 +9458,13 @@
         <v>10</v>
       </c>
       <c r="AM21" s="86" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="AN21" s="68" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="AO21" s="68" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="AP21" s="66"/>
       <c r="AQ21" s="66"/>
@@ -9476,7 +9477,7 @@
         <v>2</v>
       </c>
       <c r="AX21" s="68" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="AY21" s="70"/>
       <c r="AZ21" s="70"/>
@@ -9511,24 +9512,24 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="22" spans="1:74" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:74" ht="45" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" s="49" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="C22" s="53" t="s">
         <v>147</v>
       </c>
       <c r="D22" s="54" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="E22" s="49" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="F22" s="52" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="G22" s="55">
         <v>1968</v>
@@ -9537,10 +9538,10 @@
         <v>2001</v>
       </c>
       <c r="I22" s="55" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="J22" s="54" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="K22">
         <v>159</v>
@@ -9660,24 +9661,24 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="23" spans="1:74" ht="87" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:74" ht="105" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" s="49" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C23" s="57" t="s">
         <v>143</v>
       </c>
       <c r="D23" s="49" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="E23" s="57" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="F23" s="57" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="G23" s="56">
         <v>2009</v>
@@ -9686,10 +9687,10 @@
         <v>322</v>
       </c>
       <c r="I23" s="56" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="J23" s="49" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="K23" s="49">
         <v>2708</v>
@@ -9832,24 +9833,24 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="24" spans="1:74" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:74" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="65">
         <v>22</v>
       </c>
       <c r="B24" s="49" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="C24" s="53" t="s">
         <v>143</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>130</v>
+        <v>564</v>
       </c>
       <c r="E24" s="54" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="F24" s="53" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="G24" s="55">
         <v>2011</v>
@@ -9861,7 +9862,7 @@
         <v>330</v>
       </c>
       <c r="J24" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="K24">
         <v>499</v>
@@ -9938,7 +9939,7 @@
         <v>20</v>
       </c>
       <c r="AM24" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="AN24" s="55" t="s">
         <v>322</v>
@@ -9957,7 +9958,7 @@
         <v>1</v>
       </c>
       <c r="AX24" s="55" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="AY24" s="59"/>
       <c r="AZ24" s="59"/>
@@ -10008,24 +10009,24 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="25" spans="1:74" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:74" ht="75" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" s="49" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="C25" s="53" t="s">
         <v>143</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="E25" s="54" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="F25" s="52" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="G25" s="55">
         <v>2012</v>
@@ -10034,10 +10035,10 @@
         <v>322</v>
       </c>
       <c r="I25" s="55" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="J25" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="K25">
         <v>200</v>
@@ -10104,7 +10105,7 @@
         <v>16</v>
       </c>
       <c r="AM25" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="AN25" s="55" t="s">
         <v>322</v>
@@ -10150,24 +10151,24 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="26" spans="1:74" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:74" ht="75" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" s="49" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="C26" s="53" t="s">
         <v>143</v>
       </c>
       <c r="D26" s="53" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="E26" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="F26" s="52" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="G26" s="55">
         <v>1994</v>
@@ -10176,10 +10177,10 @@
         <v>322</v>
       </c>
       <c r="I26" s="55" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="J26" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="K26">
         <v>72.099999999999994</v>
@@ -10241,7 +10242,7 @@
         <v>11.5</v>
       </c>
       <c r="AM26" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="AN26" s="55" t="s">
         <v>322</v>
@@ -10295,24 +10296,24 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="27" spans="1:74" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:74" ht="75" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" s="49" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="C27" s="53" t="s">
         <v>143</v>
       </c>
       <c r="D27" s="53" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="E27" s="54" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="F27" s="52" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="G27" s="55">
         <v>2005</v>
@@ -10321,10 +10322,10 @@
         <v>322</v>
       </c>
       <c r="I27" s="55" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="J27" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="K27">
         <v>161</v>
@@ -10391,7 +10392,7 @@
         <v>16</v>
       </c>
       <c r="AM27" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="AN27" s="55" t="s">
         <v>322</v>
@@ -10437,24 +10438,24 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="28" spans="1:74" ht="116" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:74" ht="135" x14ac:dyDescent="0.25">
       <c r="A28" s="65">
         <v>26</v>
       </c>
       <c r="B28" s="49" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="C28" s="54" t="s">
         <v>138</v>
       </c>
       <c r="D28" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="E28" s="54" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="F28" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="G28" s="55">
         <v>2010</v>
@@ -10466,7 +10467,7 @@
         <v>323</v>
       </c>
       <c r="J28" s="54" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="K28">
         <v>7862</v>
@@ -10543,7 +10544,7 @@
         <v>14.3</v>
       </c>
       <c r="AM28" s="57" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="AN28" s="56" t="s">
         <v>322</v>
@@ -10562,18 +10563,18 @@
         <v>2</v>
       </c>
       <c r="AX28" s="60" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="AY28" s="59"/>
       <c r="AZ28" s="59"/>
       <c r="BA28" s="55" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="BB28" s="55">
         <v>0</v>
       </c>
       <c r="BC28" s="55" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="BD28" s="55">
         <v>3000</v>
@@ -10605,24 +10606,24 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="29" spans="1:74" ht="87" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:74" ht="90" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" s="49" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="C29" s="53" t="s">
         <v>138</v>
       </c>
       <c r="D29" s="53" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="E29" s="54" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="F29" s="52" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="G29" s="55">
         <v>2007</v>
@@ -10634,7 +10635,7 @@
         <v>330</v>
       </c>
       <c r="J29" s="54" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="K29">
         <v>297</v>
@@ -10705,7 +10706,7 @@
         <v>13</v>
       </c>
       <c r="AM29" s="54" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="AN29" s="55" t="s">
         <v>322</v>
@@ -10724,7 +10725,7 @@
         <v>0</v>
       </c>
       <c r="AX29" s="55" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="AY29" s="59"/>
       <c r="AZ29" s="59"/>
@@ -10751,24 +10752,24 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="30" spans="1:74" ht="58" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:74" ht="45" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" s="49" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="C30" s="53" t="s">
         <v>138</v>
       </c>
       <c r="D30" s="53" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="E30" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="F30" s="52" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="G30" s="55">
         <v>2011</v>
@@ -10777,10 +10778,10 @@
         <v>322</v>
       </c>
       <c r="I30" s="55" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="J30" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="K30">
         <v>255</v>
@@ -10847,7 +10848,7 @@
         <v>16.5</v>
       </c>
       <c r="AM30" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="AN30" s="55" t="s">
         <v>322</v>
@@ -10913,24 +10914,24 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="31" spans="1:74" ht="145" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:74" ht="165" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" s="65" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="C31" s="67" t="s">
         <v>135</v>
       </c>
       <c r="D31" s="67" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="E31" s="67" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="F31" s="66" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="G31" s="68">
         <v>2010</v>
@@ -10942,7 +10943,7 @@
         <v>323</v>
       </c>
       <c r="J31" s="66" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="K31" s="66">
         <v>7473</v>
@@ -11009,7 +11010,7 @@
       </c>
       <c r="AL31" s="66"/>
       <c r="AM31" s="67" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="AN31" s="66"/>
       <c r="AO31" s="68" t="s">
@@ -11073,24 +11074,24 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="32" spans="1:74" ht="87" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:74" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="65">
         <v>30</v>
       </c>
       <c r="B32" s="66" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="C32" s="80" t="s">
         <v>135</v>
       </c>
       <c r="D32" s="80" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="E32" s="67" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="F32" s="81" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="G32" s="68">
         <v>1996</v>
@@ -11102,7 +11103,7 @@
         <v>323</v>
       </c>
       <c r="J32" s="66" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="K32" s="66">
         <v>3588</v>
@@ -11169,7 +11170,7 @@
         <v>20</v>
       </c>
       <c r="AM32" s="67" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="AN32" s="69" t="s">
         <v>322</v>
@@ -11223,24 +11224,24 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="33" spans="1:74" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:74" ht="120" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="C33" s="53" t="s">
         <v>135</v>
       </c>
       <c r="D33" s="89" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="E33" s="54" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="F33" s="52" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="G33" s="55">
         <v>1979</v>
@@ -11252,7 +11253,7 @@
         <v>330</v>
       </c>
       <c r="J33" s="54" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="K33">
         <v>13489</v>
@@ -11363,24 +11364,24 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="34" spans="1:74" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:74" ht="75" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="C34" s="53" t="s">
         <v>130</v>
       </c>
       <c r="D34" s="53" t="s">
-        <v>130</v>
+        <v>564</v>
       </c>
       <c r="E34" s="54" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="F34" s="52" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="G34" s="55">
         <v>2007</v>
@@ -11392,7 +11393,7 @@
         <v>330</v>
       </c>
       <c r="J34" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="K34">
         <v>221</v>
@@ -11458,7 +11459,7 @@
         <v>12.05</v>
       </c>
       <c r="AM34" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="AN34" s="55"/>
       <c r="AO34" s="55" t="s">
@@ -11524,24 +11525,24 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="35" spans="1:74" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:74" ht="105" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="C35" s="53" t="s">
         <v>130</v>
       </c>
       <c r="D35" s="53" t="s">
-        <v>130</v>
+        <v>564</v>
       </c>
       <c r="E35" s="54" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="F35" s="52" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="G35" s="55">
         <v>2008</v>
@@ -11553,7 +11554,7 @@
         <v>330</v>
       </c>
       <c r="J35" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="K35">
         <v>327</v>
@@ -11618,7 +11619,7 @@
         <v>7.69</v>
       </c>
       <c r="AM35" s="54" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="AN35" s="56" t="s">
         <v>322</v>
@@ -11672,24 +11673,24 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="36" spans="1:74" ht="58" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:74" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="65">
         <v>34</v>
       </c>
       <c r="B36" s="66" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="C36" s="80" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="D36" s="80" t="s">
-        <v>130</v>
+        <v>564</v>
       </c>
       <c r="E36" s="67" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="F36" s="81" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="G36" s="68">
         <v>2008</v>
@@ -11698,10 +11699,10 @@
         <v>322</v>
       </c>
       <c r="I36" s="68" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="J36" s="66" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="K36" s="66">
         <v>221</v>
@@ -11764,7 +11765,7 @@
         <v>7.53</v>
       </c>
       <c r="AM36" s="66" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="AN36" s="69" t="s">
         <v>322</v>
@@ -11818,24 +11819,24 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="37" spans="1:74" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:74" ht="75" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="C37" s="53" t="s">
         <v>118</v>
       </c>
       <c r="D37" s="53" t="s">
-        <v>428</v>
+        <v>566</v>
       </c>
       <c r="E37" s="54" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="F37" s="53" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="G37" s="55">
         <v>2014</v>
@@ -11844,10 +11845,10 @@
         <v>322</v>
       </c>
       <c r="I37" s="55" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="J37" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="K37">
         <v>68</v>
@@ -11916,7 +11917,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="AM37" s="54" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="AN37" s="55" t="s">
         <v>322</v>
@@ -11970,24 +11971,24 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="38" spans="1:74" ht="58" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:74" ht="60" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" s="66" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="C38" s="80" t="s">
         <v>118</v>
       </c>
       <c r="D38" s="80" t="s">
-        <v>428</v>
+        <v>566</v>
       </c>
       <c r="E38" s="67" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="F38" s="80" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="G38" s="68">
         <v>2012</v>
@@ -11996,10 +11997,10 @@
         <v>322</v>
       </c>
       <c r="I38" s="68" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="J38" s="66" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="K38" s="66">
         <v>118</v>
@@ -12076,7 +12077,7 @@
         <v>7.6</v>
       </c>
       <c r="AM38" s="66" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="AN38" s="68" t="s">
         <v>322</v>
@@ -12130,24 +12131,24 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="39" spans="1:74" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:74" ht="75" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" s="66" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="C39" s="80" t="s">
         <v>118</v>
       </c>
       <c r="D39" s="80" t="s">
-        <v>428</v>
+        <v>566</v>
       </c>
       <c r="E39" s="67" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="F39" s="89" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="G39" s="68">
         <v>2013</v>
@@ -12156,10 +12157,10 @@
         <v>322</v>
       </c>
       <c r="I39" s="68" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="J39" s="66" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="K39" s="66">
         <v>20</v>
@@ -12238,7 +12239,7 @@
         <v>322</v>
       </c>
       <c r="AM39" s="82" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="AN39" s="68" t="s">
         <v>322</v>
@@ -12292,24 +12293,24 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="40" spans="1:74" ht="58" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:74" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="65">
         <v>38</v>
       </c>
       <c r="B40" s="66" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="C40" s="80" t="s">
         <v>118</v>
       </c>
       <c r="D40" s="80" t="s">
-        <v>428</v>
+        <v>566</v>
       </c>
       <c r="E40" s="67" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="F40" s="81" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="G40" s="68">
         <v>2013</v>
@@ -12318,10 +12319,10 @@
         <v>322</v>
       </c>
       <c r="I40" s="68" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="J40" s="66" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="K40" s="66">
         <v>149</v>
@@ -12398,7 +12399,7 @@
         <v>322</v>
       </c>
       <c r="AM40" s="65" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="AN40" s="69" t="s">
         <v>322</v>
@@ -12452,24 +12453,24 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="41" spans="1:74" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:74" ht="75" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" s="66" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="C41" s="80" t="s">
         <v>118</v>
       </c>
       <c r="D41" s="80" t="s">
-        <v>428</v>
+        <v>566</v>
       </c>
       <c r="E41" s="67" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="F41" s="89" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="G41" s="68">
         <v>2013</v>
@@ -12478,10 +12479,10 @@
         <v>322</v>
       </c>
       <c r="I41" s="68" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="J41" s="66" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="K41" s="66">
         <v>53</v>
@@ -12556,7 +12557,7 @@
       </c>
       <c r="AL41" s="65"/>
       <c r="AM41" s="54" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="AN41" s="68" t="s">
         <v>322</v>
@@ -12610,24 +12611,24 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="42" spans="1:74" ht="87" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:74" ht="105" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42" s="66" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="C42" s="80" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="D42" s="80" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="E42" s="67" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="F42" s="81" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="G42" s="68">
         <v>2015</v>
@@ -12636,10 +12637,10 @@
         <v>322</v>
       </c>
       <c r="I42" s="68" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="J42" s="66" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="K42" s="66"/>
       <c r="L42" s="66">
@@ -12687,7 +12688,7 @@
         <v>3</v>
       </c>
       <c r="AX42" s="69" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="AY42" s="69"/>
       <c r="AZ42" s="66"/>
@@ -12714,22 +12715,22 @@
       <c r="BU42" s="66"/>
       <c r="BV42" s="66"/>
     </row>
-    <row r="43" spans="1:74" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:74" ht="30" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43" s="66" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="C43" s="67" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="D43" s="67" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="E43" s="66"/>
       <c r="F43" s="89" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="G43" s="68">
         <v>2008</v>
@@ -12738,7 +12739,7 @@
         <v>322</v>
       </c>
       <c r="I43" s="68" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="J43" s="66"/>
       <c r="K43" s="66"/>
@@ -12806,24 +12807,24 @@
       <c r="BU43" s="66"/>
       <c r="BV43" s="66"/>
     </row>
-    <row r="44" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A44" s="65">
         <v>42</v>
       </c>
       <c r="B44" s="66" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="C44" s="80" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="D44" s="80" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="E44" s="66" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="F44" s="81" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="G44" s="68"/>
       <c r="H44" s="68" t="s">
@@ -12831,7 +12832,7 @@
       </c>
       <c r="I44" s="68"/>
       <c r="J44" s="82" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="K44" s="66"/>
       <c r="L44" s="66"/>
@@ -12908,22 +12909,22 @@
       <c r="BU44" s="66"/>
       <c r="BV44" s="66"/>
     </row>
-    <row r="45" spans="1:74" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:74" ht="30" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45" s="55" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="C45" s="92" t="s">
         <v>168</v>
       </c>
-      <c r="D45" s="92" t="s">
-        <v>551</v>
+      <c r="D45" s="146" t="s">
+        <v>546</v>
       </c>
       <c r="E45" s="55"/>
       <c r="F45" s="55" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="G45" s="55">
         <v>2012</v>
@@ -13007,13 +13008,13 @@
         <v>5.5</v>
       </c>
       <c r="AT45" s="55" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="AU45" s="55">
         <v>100</v>
       </c>
       <c r="AV45" s="55" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AW45" s="55">
         <v>2</v>
@@ -13022,11 +13023,11 @@
       <c r="AY45" s="93"/>
       <c r="AZ45" s="93"/>
       <c r="BA45" s="55" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="BB45" s="55"/>
       <c r="BC45" s="55" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="BD45" s="55"/>
       <c r="BE45" s="93"/>

</xml_diff>